<commit_message>
Moved to newest bleed. Fixed up some errors in yaml. Altered terrain movement penalty.
</commit_message>
<xml_diff>
--- a/mods/dr/The Spreadsheet.xlsx
+++ b/mods/dr/The Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{284FC09D-72BA-4B88-B4D5-DB5A308F582F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CE673801-CFD5-4400-91E1-AE9CD3C1ECAC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="528">
   <si>
     <t>Unit</t>
   </si>
@@ -1593,6 +1593,18 @@
   </si>
   <si>
     <t>Cell Size formula</t>
+  </si>
+  <si>
+    <t>FG AA</t>
+  </si>
+  <si>
+    <t>I AA</t>
+  </si>
+  <si>
+    <t>FG Laser Turret</t>
+  </si>
+  <si>
+    <t>I Plasma Turret</t>
   </si>
 </sst>
 </file>
@@ -2029,8 +2041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3782,6 +3794,9 @@
       <c r="A67" t="s">
         <v>150</v>
       </c>
+      <c r="B67" t="s">
+        <v>524</v>
+      </c>
       <c r="C67">
         <v>20</v>
       </c>
@@ -3820,6 +3835,9 @@
       <c r="A68" t="s">
         <v>157</v>
       </c>
+      <c r="B68" t="s">
+        <v>525</v>
+      </c>
       <c r="C68">
         <v>10</v>
       </c>
@@ -3982,7 +4000,7 @@
         <v>174</v>
       </c>
       <c r="B72" t="s">
-        <v>164</v>
+        <v>526</v>
       </c>
       <c r="C72">
         <v>5</v>
@@ -3994,7 +4012,7 @@
         <v>20</v>
       </c>
       <c r="F72" t="s">
-        <v>95</v>
+        <v>54</v>
       </c>
       <c r="G72">
         <v>10</v>
@@ -4003,13 +4021,13 @@
         <v>8</v>
       </c>
       <c r="I72" t="s">
-        <v>94</v>
+        <v>147</v>
       </c>
       <c r="J72" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
       <c r="K72" t="s">
-        <v>176</v>
+        <v>133</v>
       </c>
       <c r="N72" t="s">
         <v>155</v>
@@ -4020,165 +4038,162 @@
     </row>
     <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>177</v>
+        <v>290</v>
+      </c>
+      <c r="B73" t="s">
+        <v>527</v>
       </c>
       <c r="C73">
         <v>5</v>
       </c>
       <c r="D73">
+        <v>3</v>
+      </c>
+      <c r="E73">
         <v>20</v>
       </c>
-      <c r="E73">
-        <v>5</v>
-      </c>
       <c r="F73" t="s">
-        <v>179</v>
+        <v>95</v>
       </c>
       <c r="G73">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H73">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="I73" t="s">
-        <v>178</v>
+        <v>94</v>
       </c>
       <c r="J73" t="s">
-        <v>180</v>
+        <v>96</v>
       </c>
       <c r="K73" t="s">
-        <v>181</v>
+        <v>176</v>
+      </c>
+      <c r="N73" t="s">
+        <v>155</v>
       </c>
       <c r="O73" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C74">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D74">
         <v>20</v>
       </c>
       <c r="E74">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F74" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="G74">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="H74">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="I74" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="J74" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="K74" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="O74" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C75">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D75">
-        <v>10</v>
-      </c>
-      <c r="E75" s="4">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="E75">
+        <v>10</v>
       </c>
       <c r="F75" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="G75">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="H75">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="I75" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="J75" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="K75" t="s">
-        <v>194</v>
-      </c>
-      <c r="L75">
-        <v>10</v>
+        <v>188</v>
       </c>
       <c r="O75" t="s">
-        <v>190</v>
-      </c>
-      <c r="U75">
-        <v>0.5</v>
-      </c>
-      <c r="V75">
-        <v>15</v>
+        <v>184</v>
       </c>
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C76">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="D76">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="E76" s="4">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F76" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="G76">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H76">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="I76" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="J76" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="K76" t="s">
-        <v>200</v>
-      </c>
-      <c r="M76">
-        <v>3</v>
+        <v>194</v>
+      </c>
+      <c r="L76">
+        <v>10</v>
       </c>
       <c r="O76" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="U76">
-        <v>10</v>
+        <v>0.5</v>
       </c>
       <c r="V76">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="77" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C77">
         <v>45</v>
@@ -4186,8 +4201,8 @@
       <c r="D77">
         <v>80</v>
       </c>
-      <c r="E77">
-        <v>7</v>
+      <c r="E77" s="4">
+        <v>8</v>
       </c>
       <c r="F77" t="s">
         <v>198</v>
@@ -4199,68 +4214,83 @@
         <v>100</v>
       </c>
       <c r="I77" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="J77" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="K77" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="M77">
         <v>3</v>
       </c>
       <c r="O77" t="s">
-        <v>201</v>
+        <v>196</v>
+      </c>
+      <c r="U77">
+        <v>10</v>
+      </c>
+      <c r="V77">
+        <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C78">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="D78">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="E78">
-        <v>1000</v>
+        <v>7</v>
       </c>
       <c r="F78" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="G78">
-        <v>-20</v>
+        <v>30</v>
       </c>
       <c r="H78">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I78" t="s">
-        <v>127</v>
+        <v>203</v>
+      </c>
+      <c r="J78" t="s">
+        <v>204</v>
+      </c>
+      <c r="K78" t="s">
+        <v>206</v>
+      </c>
+      <c r="M78">
+        <v>3</v>
       </c>
       <c r="O78" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="79" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C79">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D79">
         <v>10</v>
       </c>
       <c r="E79">
-        <v>20</v>
+        <v>1000</v>
       </c>
       <c r="F79" t="s">
         <v>209</v>
       </c>
       <c r="G79">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="H79">
         <v>0</v>
@@ -4268,34 +4298,28 @@
       <c r="I79" t="s">
         <v>127</v>
       </c>
-      <c r="J79" t="s">
-        <v>211</v>
-      </c>
-      <c r="K79" t="s">
-        <v>212</v>
-      </c>
       <c r="O79" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="80" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C80">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D80">
         <v>10</v>
       </c>
       <c r="E80">
-        <v>1000</v>
+        <v>20</v>
       </c>
       <c r="F80" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="G80">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="H80">
         <v>0</v>
@@ -4303,228 +4327,234 @@
       <c r="I80" t="s">
         <v>127</v>
       </c>
+      <c r="J80" t="s">
+        <v>211</v>
+      </c>
+      <c r="K80" t="s">
+        <v>212</v>
+      </c>
       <c r="O80" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="81" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C81">
         <v>1</v>
       </c>
       <c r="D81">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="E81">
+        <v>1000</v>
       </c>
       <c r="F81" t="s">
-        <v>95</v>
+        <v>216</v>
       </c>
       <c r="G81">
-        <v>150</v>
+        <v>-5</v>
       </c>
       <c r="H81">
-        <v>70</v>
-      </c>
-      <c r="J81" t="s">
-        <v>217</v>
-      </c>
-      <c r="K81" t="s">
-        <v>29</v>
+        <v>0</v>
+      </c>
+      <c r="I81" t="s">
+        <v>127</v>
+      </c>
+      <c r="O81" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="82" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C82">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D82">
-        <v>10</v>
-      </c>
-      <c r="E82">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="F82" t="s">
-        <v>179</v>
+        <v>95</v>
       </c>
       <c r="G82">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="H82">
-        <v>0</v>
+        <v>70</v>
+      </c>
+      <c r="J82" t="s">
+        <v>217</v>
+      </c>
+      <c r="K82" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="83" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C83">
-        <v>350</v>
+        <v>10</v>
       </c>
       <c r="D83">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E83">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="F83" t="s">
-        <v>221</v>
+        <v>179</v>
       </c>
       <c r="G83">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H83">
-        <v>10</v>
-      </c>
-      <c r="L83">
-        <v>1</v>
-      </c>
-      <c r="N83" t="s">
-        <v>155</v>
-      </c>
-      <c r="O83" t="s">
-        <v>225</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C84">
-        <v>24</v>
+        <v>350</v>
       </c>
       <c r="D84">
-        <v>0</v>
-      </c>
-      <c r="E84" s="4">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="E84">
+        <v>100</v>
       </c>
       <c r="F84" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G84">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="H84">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="L84">
+        <v>1</v>
+      </c>
+      <c r="N84" t="s">
+        <v>155</v>
       </c>
       <c r="O84" t="s">
-        <v>224</v>
-      </c>
-      <c r="U84">
-        <v>2</v>
-      </c>
-      <c r="V84">
-        <v>10</v>
+        <v>225</v>
       </c>
     </row>
     <row r="85" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>222</v>
+      </c>
+      <c r="C85">
+        <v>24</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85" s="4">
+        <v>7</v>
+      </c>
+      <c r="F85" t="s">
+        <v>223</v>
+      </c>
+      <c r="G85">
+        <v>17</v>
+      </c>
+      <c r="H85">
+        <v>5</v>
+      </c>
+      <c r="O85" t="s">
+        <v>224</v>
+      </c>
+      <c r="U85">
+        <v>2</v>
+      </c>
+      <c r="V85">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>226</v>
       </c>
-      <c r="C85">
+      <c r="C86">
         <v>9</v>
       </c>
-      <c r="D85">
+      <c r="D86">
         <v>32</v>
       </c>
-      <c r="E85">
+      <c r="E86">
         <v>35</v>
       </c>
-      <c r="F85" t="s">
+      <c r="F86" t="s">
         <v>95</v>
       </c>
-      <c r="G85">
+      <c r="G86">
         <v>180</v>
       </c>
-      <c r="H85">
+      <c r="H86">
         <v>12</v>
       </c>
-      <c r="I85" t="s">
+      <c r="I86" t="s">
         <v>119</v>
       </c>
-      <c r="J85" t="s">
+      <c r="J86" t="s">
         <v>124</v>
       </c>
-      <c r="K85" t="s">
+      <c r="K86" t="s">
         <v>228</v>
       </c>
-      <c r="O85" t="s">
+      <c r="O86" t="s">
         <v>227</v>
-      </c>
-    </row>
-    <row r="86" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A86" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B86" t="s">
-        <v>50</v>
-      </c>
-      <c r="C86">
-        <v>1</v>
-      </c>
-      <c r="F86" t="s">
-        <v>49</v>
-      </c>
-      <c r="G86">
-        <v>10</v>
-      </c>
-      <c r="H86">
-        <v>1</v>
-      </c>
-      <c r="K86" t="s">
-        <v>51</v>
-      </c>
-      <c r="O86" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="87" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>131</v>
+        <v>48</v>
+      </c>
+      <c r="B87" t="s">
+        <v>50</v>
       </c>
       <c r="C87">
         <v>1</v>
       </c>
-      <c r="D87">
+      <c r="F87" t="s">
+        <v>49</v>
+      </c>
+      <c r="G87">
+        <v>10</v>
+      </c>
+      <c r="H87">
+        <v>1</v>
+      </c>
+      <c r="K87" t="s">
+        <v>51</v>
+      </c>
+      <c r="O87" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="88" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C88">
+        <v>1</v>
+      </c>
+      <c r="D88">
         <v>2</v>
-      </c>
-      <c r="E87">
-        <v>20</v>
-      </c>
-      <c r="F87" t="s">
-        <v>132</v>
-      </c>
-      <c r="G87">
-        <v>5</v>
-      </c>
-      <c r="H87">
-        <v>8</v>
-      </c>
-      <c r="I87" t="s">
-        <v>119</v>
-      </c>
-      <c r="K87" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="88" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C88">
-        <v>3</v>
-      </c>
-      <c r="D88">
-        <v>5</v>
       </c>
       <c r="E88">
         <v>20</v>
       </c>
       <c r="F88" t="s">
-        <v>54</v>
+        <v>132</v>
       </c>
       <c r="G88">
         <v>5</v>
@@ -4533,27 +4563,21 @@
         <v>8</v>
       </c>
       <c r="I88" t="s">
-        <v>127</v>
-      </c>
-      <c r="J88" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="K88" t="s">
-        <v>56</v>
-      </c>
-      <c r="O88" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="89" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C89">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D89">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E89">
         <v>20</v>
@@ -4562,7 +4586,7 @@
         <v>54</v>
       </c>
       <c r="G89">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H89">
         <v>8</v>
@@ -4574,44 +4598,79 @@
         <v>136</v>
       </c>
       <c r="K89" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="O89" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="90" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>90</v>
+        <v>137</v>
       </c>
       <c r="C90">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D90">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="E90">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F90" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="G90">
-        <v>170</v>
+        <v>2</v>
       </c>
       <c r="H90">
         <v>8</v>
       </c>
       <c r="I90" t="s">
-        <v>87</v>
+        <v>127</v>
       </c>
       <c r="J90" t="s">
-        <v>66</v>
+        <v>136</v>
       </c>
       <c r="K90" t="s">
         <v>89</v>
       </c>
       <c r="O90" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="91" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C91">
+        <v>7</v>
+      </c>
+      <c r="D91">
+        <v>3</v>
+      </c>
+      <c r="E91">
+        <v>40</v>
+      </c>
+      <c r="F91" t="s">
+        <v>88</v>
+      </c>
+      <c r="G91">
+        <v>170</v>
+      </c>
+      <c r="H91">
+        <v>8</v>
+      </c>
+      <c r="I91" t="s">
+        <v>87</v>
+      </c>
+      <c r="J91" t="s">
+        <v>66</v>
+      </c>
+      <c r="K91" t="s">
+        <v>89</v>
+      </c>
+      <c r="O91" t="s">
         <v>91</v>
       </c>
     </row>
@@ -6871,8 +6930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD92D53-EC10-4CE0-957A-62D9B9206E5C}">
   <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7572,7 +7631,7 @@
       </c>
       <c r="F29" t="str">
         <f>Source!F72</f>
-        <v>E3</v>
+        <v>E2</v>
       </c>
       <c r="G29">
         <f>Source!G72</f>
@@ -7582,7 +7641,7 @@
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>Source!A73</f>
-        <v>PolyAcid</v>
+        <v>GatPlasma</v>
       </c>
       <c r="B30">
         <f>Source!C73 * Results!$B$6</f>
@@ -7590,33 +7649,33 @@
       </c>
       <c r="C30">
         <f>Source!D73*Results!$B$4</f>
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="D30" s="8">
         <f>Source!E73*Results!$B$3</f>
-        <v>213.33333333333331</v>
+        <v>853.33333333333326</v>
       </c>
       <c r="E30">
         <f>Source!H73*Results!$B$5</f>
-        <v>192</v>
+        <v>64</v>
       </c>
       <c r="F30" t="str">
         <f>Source!F73</f>
-        <v>M3</v>
+        <v>E3</v>
       </c>
       <c r="G30">
         <f>Source!G73</f>
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>Source!A74</f>
-        <v>TankHunterGun</v>
+        <v>PolyAcid</v>
       </c>
       <c r="B31">
         <f>Source!C74 * Results!$B$6</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C31">
         <f>Source!D74*Results!$B$4</f>
@@ -7624,85 +7683,85 @@
       </c>
       <c r="D31" s="8">
         <f>Source!E74*Results!$B$3</f>
-        <v>426.66666666666663</v>
+        <v>213.33333333333331</v>
       </c>
       <c r="E31">
         <f>Source!H74*Results!$B$5</f>
-        <v>64</v>
+        <v>192</v>
       </c>
       <c r="F31" t="str">
         <f>Source!F74</f>
-        <v>E5</v>
+        <v>M3</v>
       </c>
       <c r="G31">
         <f>Source!G74</f>
-        <v>60</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f>Source!A75</f>
-        <v>OutriderMissile</v>
+        <v>TankHunterGun</v>
       </c>
       <c r="B32">
         <f>Source!C75 * Results!$B$6</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C32">
         <f>Source!D75*Results!$B$4</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D32" s="8">
         <f>Source!E75*Results!$B$3</f>
-        <v>554.66666666666663</v>
+        <v>426.66666666666663</v>
       </c>
       <c r="E32">
         <f>Source!H75*Results!$B$5</f>
-        <v>320</v>
+        <v>64</v>
       </c>
       <c r="F32" t="str">
         <f>Source!F75</f>
-        <v>M1</v>
+        <v>E5</v>
       </c>
       <c r="G32">
         <f>Source!G75</f>
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>Source!A76</f>
-        <v>ArtilleryShell</v>
+        <v>OutriderMissile</v>
       </c>
       <c r="B33">
         <f>Source!C76 * Results!$B$6</f>
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C33">
         <f>Source!D76*Results!$B$4</f>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="D33" s="8">
         <f>Source!E76*Results!$B$3</f>
-        <v>341.33333333333331</v>
+        <v>554.66666666666663</v>
       </c>
       <c r="E33">
         <f>Source!H76*Results!$B$5</f>
-        <v>800</v>
+        <v>320</v>
       </c>
       <c r="F33" t="str">
         <f>Source!F76</f>
-        <v>K2</v>
+        <v>M1</v>
       </c>
       <c r="G33">
         <f>Source!G76</f>
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f>Source!A77</f>
-        <v>IMPArtilleryShell</v>
+        <v>ArtilleryShell</v>
       </c>
       <c r="B34">
         <f>Source!C77 * Results!$B$6</f>
@@ -7714,7 +7773,7 @@
       </c>
       <c r="D34" s="8">
         <f>Source!E77*Results!$B$3</f>
-        <v>298.66666666666663</v>
+        <v>341.33333333333331</v>
       </c>
       <c r="E34">
         <f>Source!H77*Results!$B$5</f>
@@ -7732,41 +7791,41 @@
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f>Source!A78</f>
-        <v>MedicHeal</v>
+        <v>IMPArtilleryShell</v>
       </c>
       <c r="B35">
         <f>Source!C78 * Results!$B$6</f>
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="C35">
         <f>Source!D78*Results!$B$4</f>
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="D35" s="8">
         <f>Source!E78*Results!$B$3</f>
-        <v>42666.666666666664</v>
+        <v>298.66666666666663</v>
       </c>
       <c r="E35">
         <f>Source!H78*Results!$B$5</f>
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="F35" t="str">
         <f>Source!F78</f>
-        <v>H1</v>
+        <v>K2</v>
       </c>
       <c r="G35">
         <f>Source!G78</f>
-        <v>-20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f>Source!A79</f>
-        <v>AmperAmp</v>
+        <v>MedicHeal</v>
       </c>
       <c r="B36">
         <f>Source!C79 * Results!$B$6</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C36">
         <f>Source!D79*Results!$B$4</f>
@@ -7774,7 +7833,7 @@
       </c>
       <c r="D36" s="8">
         <f>Source!E79*Results!$B$3</f>
-        <v>853.33333333333326</v>
+        <v>42666.666666666664</v>
       </c>
       <c r="E36">
         <f>Source!H79*Results!$B$5</f>
@@ -7786,17 +7845,17 @@
       </c>
       <c r="G36">
         <f>Source!G79</f>
-        <v>0</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f>Source!A80</f>
-        <v>MechanicRepair</v>
+        <v>AmperAmp</v>
       </c>
       <c r="B37">
         <f>Source!C80 * Results!$B$6</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C37">
         <f>Source!D80*Results!$B$4</f>
@@ -7804,7 +7863,7 @@
       </c>
       <c r="D37" s="8">
         <f>Source!E80*Results!$B$3</f>
-        <v>42666.666666666664</v>
+        <v>853.33333333333326</v>
       </c>
       <c r="E37">
         <f>Source!H80*Results!$B$5</f>
@@ -7812,17 +7871,17 @@
       </c>
       <c r="F37" t="str">
         <f>Source!F80</f>
-        <v>R1</v>
+        <v>H1</v>
       </c>
       <c r="G37">
         <f>Source!G80</f>
-        <v>-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f>Source!A81</f>
-        <v>SelfDestruct1</v>
+        <v>MechanicRepair</v>
       </c>
       <c r="B38">
         <f>Source!C81 * Results!$B$6</f>
@@ -7830,143 +7889,143 @@
       </c>
       <c r="C38">
         <f>Source!D81*Results!$B$4</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D38" s="8">
         <f>Source!E81*Results!$B$3</f>
-        <v>0</v>
+        <v>42666.666666666664</v>
       </c>
       <c r="E38">
         <f>Source!H81*Results!$B$5</f>
-        <v>560</v>
+        <v>0</v>
       </c>
       <c r="F38" t="str">
         <f>Source!F81</f>
-        <v>E3</v>
+        <v>R1</v>
       </c>
       <c r="G38">
         <f>Source!G81</f>
-        <v>150</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f>Source!A82</f>
-        <v>NoWeapon</v>
+        <v>SelfDestruct1</v>
       </c>
       <c r="B39">
         <f>Source!C82 * Results!$B$6</f>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C39">
         <f>Source!D82*Results!$B$4</f>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D39" s="8">
         <f>Source!E82*Results!$B$3</f>
-        <v>42666.666666666664</v>
+        <v>0</v>
       </c>
       <c r="E39">
         <f>Source!H82*Results!$B$5</f>
-        <v>0</v>
+        <v>560</v>
       </c>
       <c r="F39" t="str">
         <f>Source!F82</f>
-        <v>M3</v>
+        <v>E3</v>
       </c>
       <c r="G39">
         <f>Source!G82</f>
-        <v>0</v>
+        <v>150</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f>Source!A83</f>
-        <v>TemporalRift</v>
+        <v>NoWeapon</v>
       </c>
       <c r="B40">
         <f>Source!C83 * Results!$B$6</f>
-        <v>350</v>
+        <v>10</v>
       </c>
       <c r="C40">
         <f>Source!D83*Results!$B$4</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D40" s="8">
         <f>Source!E83*Results!$B$3</f>
-        <v>4266.6666666666661</v>
+        <v>42666.666666666664</v>
       </c>
       <c r="E40">
         <f>Source!H83*Results!$B$5</f>
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="F40" t="str">
         <f>Source!F83</f>
-        <v>V1</v>
+        <v>M3</v>
       </c>
       <c r="G40">
         <f>Source!G83</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f>Source!A84</f>
-        <v>SeismicWave</v>
+        <v>TemporalRift</v>
       </c>
       <c r="B41">
         <f>Source!C84 * Results!$B$6</f>
-        <v>24</v>
+        <v>350</v>
       </c>
       <c r="C41">
         <f>Source!D84*Results!$B$4</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41" s="8">
         <f>Source!E84*Results!$B$3</f>
-        <v>298.66666666666663</v>
+        <v>4266.6666666666661</v>
       </c>
       <c r="E41">
         <f>Source!H84*Results!$B$5</f>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="F41" t="str">
         <f>Source!F84</f>
-        <v>W1</v>
+        <v>V1</v>
       </c>
       <c r="G41">
         <f>Source!G84</f>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f>Source!A85</f>
-        <v>NeutronAss</v>
+        <v>SeismicWave</v>
       </c>
       <c r="B42">
         <f>Source!C85 * Results!$B$6</f>
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C42">
         <f>Source!D85*Results!$B$4</f>
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="D42" s="8">
         <f>Source!E85*Results!$B$3</f>
-        <v>1493.3333333333333</v>
+        <v>298.66666666666663</v>
       </c>
       <c r="E42">
         <f>Source!H85*Results!$B$5</f>
-        <v>96</v>
+        <v>40</v>
       </c>
       <c r="F42" t="str">
         <f>Source!F85</f>
-        <v>E3</v>
+        <v>W1</v>
       </c>
       <c r="G42">
         <f>Source!G85</f>
-        <v>180</v>
+        <v>17</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added shadows to a lot of objects and buildings. Let RAT and ITT move units. Corrected IMP plasma turret sounds and sprites. Removed 6chemy map. Added two new 8 player maps.
</commit_message>
<xml_diff>
--- a/mods/dr/The Spreadsheet.xlsx
+++ b/mods/dr/The Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CE673801-CFD5-4400-91E1-AE9CD3C1ECAC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{21D69477-E333-4529-8CC7-8E3BA8C2E6F7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -515,9 +515,6 @@
     <t>This Weapon is used by the Freedom Guard Heavy Laser Platform</t>
   </si>
   <si>
-    <t>???? Is this used?</t>
-  </si>
-  <si>
     <t>gxfagwc0</t>
   </si>
   <si>
@@ -1605,6 +1602,9 @@
   </si>
   <si>
     <t>I Plasma Turret</t>
+  </si>
+  <si>
+    <t>FG Rail Turret</t>
   </si>
 </sst>
 </file>
@@ -2041,8 +2041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2063,7 +2063,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -2101,13 +2101,13 @@
         <v>32</v>
       </c>
       <c r="K10" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="L10" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="L10" s="5" t="s">
-        <v>310</v>
-      </c>
       <c r="M10" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -2118,10 +2118,10 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
+        <v>228</v>
+      </c>
+      <c r="D11" t="s">
         <v>229</v>
-      </c>
-      <c r="D11" t="s">
-        <v>230</v>
       </c>
       <c r="E11">
         <v>1450</v>
@@ -2147,10 +2147,10 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
+        <v>228</v>
+      </c>
+      <c r="D12" t="s">
         <v>229</v>
-      </c>
-      <c r="D12" t="s">
-        <v>230</v>
       </c>
       <c r="E12">
         <v>1450</v>
@@ -2208,7 +2208,7 @@
         <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E14">
         <v>1300</v>
@@ -2237,7 +2237,7 @@
         <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E15">
         <v>1200</v>
@@ -2257,16 +2257,16 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
       </c>
       <c r="C16" t="s">
+        <v>275</v>
+      </c>
+      <c r="D16" t="s">
         <v>276</v>
-      </c>
-      <c r="D16" t="s">
-        <v>277</v>
       </c>
       <c r="E16">
         <v>2400</v>
@@ -2286,16 +2286,16 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
       </c>
       <c r="C17" t="s">
+        <v>277</v>
+      </c>
+      <c r="D17" t="s">
         <v>278</v>
-      </c>
-      <c r="D17" t="s">
-        <v>279</v>
       </c>
       <c r="E17">
         <v>3600</v>
@@ -2321,10 +2321,10 @@
         <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E18" s="1">
         <v>1440</v>
@@ -2344,16 +2344,16 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B19" t="s">
         <v>11</v>
       </c>
       <c r="C19" t="s">
+        <v>270</v>
+      </c>
+      <c r="D19" t="s">
         <v>271</v>
-      </c>
-      <c r="D19" t="s">
-        <v>272</v>
       </c>
       <c r="E19" s="1">
         <v>2880</v>
@@ -2373,16 +2373,16 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
       </c>
       <c r="C20" t="s">
+        <v>272</v>
+      </c>
+      <c r="D20" t="s">
         <v>273</v>
-      </c>
-      <c r="D20" t="s">
-        <v>274</v>
       </c>
       <c r="E20" s="1">
         <v>4330</v>
@@ -2408,10 +2408,10 @@
         <v>12</v>
       </c>
       <c r="C21" t="s">
+        <v>230</v>
+      </c>
+      <c r="D21" t="s">
         <v>231</v>
-      </c>
-      <c r="D21" t="s">
-        <v>232</v>
       </c>
       <c r="E21">
         <v>750</v>
@@ -2431,16 +2431,16 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B22" t="s">
         <v>12</v>
       </c>
       <c r="C22" t="s">
+        <v>233</v>
+      </c>
+      <c r="D22" t="s">
         <v>234</v>
-      </c>
-      <c r="D22" t="s">
-        <v>235</v>
       </c>
       <c r="E22">
         <v>1500</v>
@@ -2466,10 +2466,10 @@
         <v>11</v>
       </c>
       <c r="C23" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D23" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E23" s="1">
         <v>900</v>
@@ -2489,16 +2489,16 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B24" t="s">
         <v>11</v>
       </c>
       <c r="C24" t="s">
+        <v>281</v>
+      </c>
+      <c r="D24" t="s">
         <v>282</v>
-      </c>
-      <c r="D24" t="s">
-        <v>283</v>
       </c>
       <c r="E24" s="1">
         <v>1800</v>
@@ -2524,10 +2524,10 @@
         <v>10</v>
       </c>
       <c r="C25" t="s">
+        <v>236</v>
+      </c>
+      <c r="D25" t="s">
         <v>237</v>
-      </c>
-      <c r="D25" t="s">
-        <v>238</v>
       </c>
       <c r="E25">
         <v>1000</v>
@@ -2547,16 +2547,16 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
       </c>
       <c r="C26" t="s">
+        <v>238</v>
+      </c>
+      <c r="D26" t="s">
         <v>239</v>
-      </c>
-      <c r="D26" t="s">
-        <v>240</v>
       </c>
       <c r="E26">
         <v>2000</v>
@@ -2582,10 +2582,10 @@
         <v>11</v>
       </c>
       <c r="C27" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D27" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E27" s="1">
         <v>1200</v>
@@ -2605,16 +2605,16 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B28" t="s">
         <v>11</v>
       </c>
       <c r="C28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D28" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E28" s="1">
         <v>2400</v>
@@ -2640,10 +2640,10 @@
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D29" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E29">
         <v>400</v>
@@ -2661,16 +2661,16 @@
         <v>29</v>
       </c>
       <c r="J29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K29" t="s">
+        <v>241</v>
+      </c>
+      <c r="L29" t="s">
         <v>242</v>
       </c>
-      <c r="L29" t="s">
-        <v>243</v>
-      </c>
       <c r="M29" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -2681,10 +2681,10 @@
         <v>11</v>
       </c>
       <c r="C30" t="s">
+        <v>287</v>
+      </c>
+      <c r="D30" t="s">
         <v>288</v>
-      </c>
-      <c r="D30" t="s">
-        <v>289</v>
       </c>
       <c r="E30">
         <v>400</v>
@@ -2702,16 +2702,16 @@
         <v>29</v>
       </c>
       <c r="J30" t="s">
+        <v>289</v>
+      </c>
+      <c r="K30" t="s">
         <v>290</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>291</v>
       </c>
-      <c r="L30" t="s">
-        <v>292</v>
-      </c>
       <c r="M30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -2722,10 +2722,10 @@
         <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D31" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E31">
         <v>600</v>
@@ -2754,10 +2754,10 @@
         <v>11</v>
       </c>
       <c r="C32" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D32" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E32" s="1">
         <v>720</v>
@@ -2786,10 +2786,10 @@
         <v>10</v>
       </c>
       <c r="C33" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D33" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E33">
         <v>550</v>
@@ -2818,10 +2818,10 @@
         <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D34" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E34">
         <v>550</v>
@@ -2839,16 +2839,16 @@
         <v>29</v>
       </c>
       <c r="J34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K34" t="s">
+        <v>294</v>
+      </c>
+      <c r="L34" t="s">
         <v>295</v>
       </c>
-      <c r="L34" t="s">
-        <v>296</v>
-      </c>
       <c r="M34" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -2859,10 +2859,10 @@
         <v>10</v>
       </c>
       <c r="C35" t="s">
+        <v>254</v>
+      </c>
+      <c r="D35" t="s">
         <v>255</v>
-      </c>
-      <c r="D35" t="s">
-        <v>256</v>
       </c>
       <c r="E35">
         <v>600</v>
@@ -2888,10 +2888,10 @@
         <v>11</v>
       </c>
       <c r="C36" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D36" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E36" s="1">
         <v>720</v>
@@ -2917,10 +2917,10 @@
         <v>10</v>
       </c>
       <c r="C37" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D37" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E37">
         <v>600</v>
@@ -2946,10 +2946,10 @@
         <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D38" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E38" s="1">
         <v>720</v>
@@ -2975,10 +2975,10 @@
         <v>10</v>
       </c>
       <c r="C39" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D39" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E39">
         <v>800</v>
@@ -3004,10 +3004,10 @@
         <v>11</v>
       </c>
       <c r="C40" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D40" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E40" s="1">
         <v>960</v>
@@ -3033,10 +3033,10 @@
         <v>10</v>
       </c>
       <c r="C41" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D41" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E41">
         <v>1000</v>
@@ -3056,16 +3056,16 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>260</v>
+      </c>
+      <c r="B42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" t="s">
         <v>261</v>
       </c>
-      <c r="B42" t="s">
-        <v>10</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>262</v>
-      </c>
-      <c r="D42" t="s">
-        <v>263</v>
       </c>
       <c r="E42">
         <v>2000</v>
@@ -3091,10 +3091,10 @@
         <v>11</v>
       </c>
       <c r="C43" t="s">
+        <v>302</v>
+      </c>
+      <c r="D43" t="s">
         <v>303</v>
-      </c>
-      <c r="D43" t="s">
-        <v>304</v>
       </c>
       <c r="E43">
         <v>1000</v>
@@ -3120,10 +3120,10 @@
         <v>11</v>
       </c>
       <c r="C44" t="s">
+        <v>306</v>
+      </c>
+      <c r="D44" t="s">
         <v>307</v>
-      </c>
-      <c r="D44" t="s">
-        <v>308</v>
       </c>
       <c r="E44">
         <v>1000</v>
@@ -3146,10 +3146,10 @@
         <v>130</v>
       </c>
       <c r="C45" t="s">
+        <v>251</v>
+      </c>
+      <c r="D45" t="s">
         <v>252</v>
-      </c>
-      <c r="D45" t="s">
-        <v>253</v>
       </c>
       <c r="E45">
         <v>150</v>
@@ -3164,12 +3164,12 @@
         <v>6</v>
       </c>
       <c r="I45" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="51" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3220,10 +3220,10 @@
       </c>
       <c r="P51" s="5"/>
       <c r="U51" t="s">
+        <v>520</v>
+      </c>
+      <c r="V51" t="s">
         <v>521</v>
-      </c>
-      <c r="V51" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
@@ -3795,9 +3795,9 @@
         <v>150</v>
       </c>
       <c r="B67" t="s">
-        <v>524</v>
-      </c>
-      <c r="C67">
+        <v>523</v>
+      </c>
+      <c r="C67" s="1">
         <v>20</v>
       </c>
       <c r="D67">
@@ -3809,7 +3809,7 @@
       <c r="F67" t="s">
         <v>153</v>
       </c>
-      <c r="G67">
+      <c r="G67" s="1">
         <v>40</v>
       </c>
       <c r="H67">
@@ -3836,7 +3836,7 @@
         <v>157</v>
       </c>
       <c r="B68" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C68">
         <v>10</v>
@@ -3877,7 +3877,7 @@
         <v>162</v>
       </c>
       <c r="B69" t="s">
-        <v>164</v>
+        <v>527</v>
       </c>
       <c r="C69">
         <v>9</v>
@@ -3904,7 +3904,7 @@
         <v>61</v>
       </c>
       <c r="K69" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="O69" t="s">
         <v>163</v>
@@ -3912,7 +3912,7 @@
     </row>
     <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C70">
         <v>8</v>
@@ -3939,18 +3939,18 @@
         <v>160</v>
       </c>
       <c r="K70" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="N70" t="s">
         <v>155</v>
       </c>
       <c r="O70" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C71">
         <v>5</v>
@@ -3971,13 +3971,13 @@
         <v>10</v>
       </c>
       <c r="I71" t="s">
+        <v>170</v>
+      </c>
+      <c r="J71" t="s">
         <v>171</v>
       </c>
-      <c r="J71" t="s">
+      <c r="K71" t="s">
         <v>172</v>
-      </c>
-      <c r="K71" t="s">
-        <v>173</v>
       </c>
       <c r="L71">
         <v>20</v>
@@ -3986,7 +3986,7 @@
         <v>155</v>
       </c>
       <c r="O71" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="U71">
         <v>1</v>
@@ -3997,10 +3997,10 @@
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B72" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C72">
         <v>5</v>
@@ -4033,15 +4033,15 @@
         <v>155</v>
       </c>
       <c r="O72" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B73" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C73">
         <v>5</v>
@@ -4068,18 +4068,18 @@
         <v>96</v>
       </c>
       <c r="K73" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="N73" t="s">
         <v>155</v>
       </c>
       <c r="O73" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C74">
         <v>5</v>
@@ -4091,7 +4091,7 @@
         <v>5</v>
       </c>
       <c r="F74" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G74">
         <v>15</v>
@@ -4100,21 +4100,21 @@
         <v>24</v>
       </c>
       <c r="I74" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J74" t="s">
+        <v>179</v>
+      </c>
+      <c r="K74" t="s">
         <v>180</v>
       </c>
-      <c r="K74" t="s">
+      <c r="O74" t="s">
         <v>181</v>
-      </c>
-      <c r="O74" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C75">
         <v>3</v>
@@ -4126,7 +4126,7 @@
         <v>10</v>
       </c>
       <c r="F75" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G75">
         <v>60</v>
@@ -4135,21 +4135,21 @@
         <v>8</v>
       </c>
       <c r="I75" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J75" t="s">
+        <v>186</v>
+      </c>
+      <c r="K75" t="s">
         <v>187</v>
       </c>
-      <c r="K75" t="s">
-        <v>188</v>
-      </c>
       <c r="O75" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C76">
         <v>5</v>
@@ -4161,7 +4161,7 @@
         <v>13</v>
       </c>
       <c r="F76" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G76">
         <v>20</v>
@@ -4170,19 +4170,19 @@
         <v>40</v>
       </c>
       <c r="I76" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J76" t="s">
+        <v>192</v>
+      </c>
+      <c r="K76" t="s">
         <v>193</v>
       </c>
-      <c r="K76" t="s">
-        <v>194</v>
-      </c>
       <c r="L76">
         <v>10</v>
       </c>
       <c r="O76" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="U76">
         <v>0.5</v>
@@ -4193,7 +4193,7 @@
     </row>
     <row r="77" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C77">
         <v>45</v>
@@ -4205,7 +4205,7 @@
         <v>8</v>
       </c>
       <c r="F77" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G77">
         <v>30</v>
@@ -4214,19 +4214,19 @@
         <v>100</v>
       </c>
       <c r="I77" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J77" t="s">
+        <v>198</v>
+      </c>
+      <c r="K77" t="s">
         <v>199</v>
-      </c>
-      <c r="K77" t="s">
-        <v>200</v>
       </c>
       <c r="M77">
         <v>3</v>
       </c>
       <c r="O77" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="U77">
         <v>10</v>
@@ -4237,7 +4237,7 @@
     </row>
     <row r="78" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C78">
         <v>45</v>
@@ -4249,7 +4249,7 @@
         <v>7</v>
       </c>
       <c r="F78" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G78">
         <v>30</v>
@@ -4258,24 +4258,24 @@
         <v>100</v>
       </c>
       <c r="I78" t="s">
+        <v>202</v>
+      </c>
+      <c r="J78" t="s">
         <v>203</v>
       </c>
-      <c r="J78" t="s">
-        <v>204</v>
-      </c>
       <c r="K78" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M78">
         <v>3</v>
       </c>
       <c r="O78" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="79" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C79">
         <v>1</v>
@@ -4287,7 +4287,7 @@
         <v>1000</v>
       </c>
       <c r="F79" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G79">
         <v>-20</v>
@@ -4299,12 +4299,12 @@
         <v>127</v>
       </c>
       <c r="O79" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="80" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C80">
         <v>5</v>
@@ -4316,7 +4316,7 @@
         <v>20</v>
       </c>
       <c r="F80" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G80">
         <v>0</v>
@@ -4328,18 +4328,18 @@
         <v>127</v>
       </c>
       <c r="J80" t="s">
+        <v>210</v>
+      </c>
+      <c r="K80" t="s">
         <v>211</v>
       </c>
-      <c r="K80" t="s">
+      <c r="O80" t="s">
         <v>212</v>
-      </c>
-      <c r="O80" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="81" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C81">
         <v>1</v>
@@ -4351,7 +4351,7 @@
         <v>1000</v>
       </c>
       <c r="F81" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G81">
         <v>-5</v>
@@ -4363,12 +4363,12 @@
         <v>127</v>
       </c>
       <c r="O81" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="82" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -4386,7 +4386,7 @@
         <v>70</v>
       </c>
       <c r="J82" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K82" t="s">
         <v>29</v>
@@ -4394,7 +4394,7 @@
     </row>
     <row r="83" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C83">
         <v>10</v>
@@ -4406,7 +4406,7 @@
         <v>1000</v>
       </c>
       <c r="F83" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -4417,7 +4417,7 @@
     </row>
     <row r="84" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C84">
         <v>350</v>
@@ -4429,7 +4429,7 @@
         <v>100</v>
       </c>
       <c r="F84" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G84">
         <v>4</v>
@@ -4444,12 +4444,12 @@
         <v>155</v>
       </c>
       <c r="O84" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="85" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C85">
         <v>24</v>
@@ -4461,7 +4461,7 @@
         <v>7</v>
       </c>
       <c r="F85" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G85">
         <v>17</v>
@@ -4470,7 +4470,7 @@
         <v>5</v>
       </c>
       <c r="O85" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="U85">
         <v>2</v>
@@ -4481,7 +4481,7 @@
     </row>
     <row r="86" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C86">
         <v>9</v>
@@ -4508,10 +4508,10 @@
         <v>124</v>
       </c>
       <c r="K86" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O86" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="87" spans="1:22" x14ac:dyDescent="0.25">
@@ -4694,7 +4694,7 @@
         <v>4</v>
       </c>
       <c r="G95" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H95" s="5" t="s">
         <v>27</v>
@@ -4703,42 +4703,42 @@
         <v>5</v>
       </c>
       <c r="J95" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="K95" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="L95" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="M95" s="7" t="s">
         <v>317</v>
       </c>
-      <c r="M95" s="7" t="s">
-        <v>318</v>
-      </c>
       <c r="O95" s="7" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="Q95" s="7" t="s">
         <v>32</v>
       </c>
       <c r="S95" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="T95" t="s">
+        <v>407</v>
+      </c>
+      <c r="U95" t="s">
         <v>408</v>
       </c>
-      <c r="U95" t="s">
-        <v>409</v>
-      </c>
       <c r="V95" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="96" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B96" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C96" t="s">
         <v>10</v>
@@ -4759,10 +4759,10 @@
         <v>9</v>
       </c>
       <c r="I96" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="J96" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="K96">
         <v>30</v>
@@ -4773,10 +4773,10 @@
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
+        <v>321</v>
+      </c>
+      <c r="B97" t="s">
         <v>322</v>
-      </c>
-      <c r="B97" t="s">
-        <v>323</v>
       </c>
       <c r="C97" t="s">
         <v>10</v>
@@ -4797,10 +4797,10 @@
         <v>9</v>
       </c>
       <c r="I97" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="J97" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="K97">
         <v>10</v>
@@ -4811,10 +4811,10 @@
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B98" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C98" t="s">
         <v>10</v>
@@ -4835,10 +4835,10 @@
         <v>9</v>
       </c>
       <c r="I98" t="s">
+        <v>334</v>
+      </c>
+      <c r="J98" t="s">
         <v>335</v>
-      </c>
-      <c r="J98" t="s">
-        <v>336</v>
       </c>
       <c r="K98">
         <v>10</v>
@@ -4850,7 +4850,7 @@
         <v>52</v>
       </c>
       <c r="R98" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="U98" t="s">
         <v>155</v>
@@ -4858,10 +4858,10 @@
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B99" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C99" t="s">
         <v>10</v>
@@ -4882,10 +4882,10 @@
         <v>8</v>
       </c>
       <c r="I99" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="J99" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="K99">
         <v>30</v>
@@ -4899,10 +4899,10 @@
     </row>
     <row r="100" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>327</v>
+      </c>
+      <c r="B100" t="s">
         <v>328</v>
-      </c>
-      <c r="B100" t="s">
-        <v>329</v>
       </c>
       <c r="C100" t="s">
         <v>10</v>
@@ -4923,10 +4923,10 @@
         <v>8</v>
       </c>
       <c r="I100" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="J100" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="K100">
         <v>30</v>
@@ -4940,10 +4940,10 @@
     </row>
     <row r="101" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B101" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C101" t="s">
         <v>10</v>
@@ -4964,10 +4964,10 @@
         <v>12</v>
       </c>
       <c r="I101" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="J101" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="K101">
         <v>30</v>
@@ -4978,10 +4978,10 @@
     </row>
     <row r="102" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B102" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C102" t="s">
         <v>10</v>
@@ -5002,10 +5002,10 @@
         <v>12</v>
       </c>
       <c r="I102" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J102" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="K102">
         <v>30</v>
@@ -5013,10 +5013,10 @@
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
+        <v>347</v>
+      </c>
+      <c r="B103" t="s">
         <v>348</v>
-      </c>
-      <c r="B103" t="s">
-        <v>349</v>
       </c>
       <c r="C103" t="s">
         <v>10</v>
@@ -5037,10 +5037,10 @@
         <v>8</v>
       </c>
       <c r="I103" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="J103" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K103">
         <v>30</v>
@@ -5049,15 +5049,15 @@
         <v>51</v>
       </c>
       <c r="Q103" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B104" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C104" t="s">
         <v>10</v>
@@ -5078,10 +5078,10 @@
         <v>9</v>
       </c>
       <c r="I104" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="J104" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="K104">
         <v>30</v>
@@ -5092,10 +5092,10 @@
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B105" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C105" t="s">
         <v>10</v>
@@ -5116,10 +5116,10 @@
         <v>8</v>
       </c>
       <c r="I105" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J105" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K105">
         <v>30</v>
@@ -5128,15 +5128,15 @@
         <v>51</v>
       </c>
       <c r="Q105" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="106" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B106" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C106" t="s">
         <v>10</v>
@@ -5157,10 +5157,10 @@
         <v>8</v>
       </c>
       <c r="I106" t="s">
+        <v>361</v>
+      </c>
+      <c r="J106" t="s">
         <v>362</v>
-      </c>
-      <c r="J106" t="s">
-        <v>363</v>
       </c>
       <c r="K106">
         <v>30</v>
@@ -5171,10 +5171,10 @@
     </row>
     <row r="107" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B107" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D107">
         <v>1000</v>
@@ -5192,10 +5192,10 @@
         <v>9</v>
       </c>
       <c r="I107" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="J107" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="K107">
         <v>30</v>
@@ -5206,10 +5206,10 @@
     </row>
     <row r="108" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
+        <v>368</v>
+      </c>
+      <c r="B108" t="s">
         <v>369</v>
-      </c>
-      <c r="B108" t="s">
-        <v>370</v>
       </c>
       <c r="C108" t="s">
         <v>10</v>
@@ -5230,10 +5230,10 @@
         <v>9</v>
       </c>
       <c r="I108" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="J108" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="K108">
         <v>10</v>
@@ -5247,10 +5247,10 @@
     </row>
     <row r="109" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B109" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C109" t="s">
         <v>10</v>
@@ -5271,10 +5271,10 @@
         <v>9</v>
       </c>
       <c r="I109" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J109" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="K109">
         <v>12</v>
@@ -5283,7 +5283,7 @@
         <v>51</v>
       </c>
       <c r="S109" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="U109" t="s">
         <v>155</v>
@@ -5291,10 +5291,10 @@
     </row>
     <row r="110" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B110" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C110" t="s">
         <v>10</v>
@@ -5315,10 +5315,10 @@
         <v>9</v>
       </c>
       <c r="I110" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="J110" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="K110">
         <v>10</v>
@@ -5330,18 +5330,18 @@
         <v>80</v>
       </c>
       <c r="T110" t="s">
+        <v>381</v>
+      </c>
+      <c r="U110" t="s">
         <v>382</v>
-      </c>
-      <c r="U110" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="111" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B111" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C111" t="s">
         <v>10</v>
@@ -5362,10 +5362,10 @@
         <v>9</v>
       </c>
       <c r="I111" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="J111" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="K111">
         <v>30</v>
@@ -5374,15 +5374,15 @@
         <v>51</v>
       </c>
       <c r="Q111" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="112" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B112" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C112" t="s">
         <v>10</v>
@@ -5403,10 +5403,10 @@
         <v>9</v>
       </c>
       <c r="I112" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="J112" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="K112">
         <v>10</v>
@@ -5420,10 +5420,10 @@
     </row>
     <row r="113" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B113" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C113" t="s">
         <v>10</v>
@@ -5444,10 +5444,10 @@
         <v>9</v>
       </c>
       <c r="I113" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J113" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="K113">
         <v>30</v>
@@ -5461,10 +5461,10 @@
     </row>
     <row r="114" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B114" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C114" t="s">
         <v>10</v>
@@ -5485,10 +5485,10 @@
         <v>9</v>
       </c>
       <c r="I114" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="J114" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="K114">
         <v>10</v>
@@ -5500,7 +5500,7 @@
         <v>75</v>
       </c>
       <c r="T114" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="U114" t="s">
         <v>155</v>
@@ -5508,10 +5508,10 @@
     </row>
     <row r="115" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
+        <v>401</v>
+      </c>
+      <c r="B115" t="s">
         <v>402</v>
-      </c>
-      <c r="B115" t="s">
-        <v>403</v>
       </c>
       <c r="C115" t="s">
         <v>10</v>
@@ -5532,10 +5532,10 @@
         <v>9</v>
       </c>
       <c r="I115" t="s">
+        <v>403</v>
+      </c>
+      <c r="J115" t="s">
         <v>404</v>
-      </c>
-      <c r="J115" t="s">
-        <v>405</v>
       </c>
       <c r="K115">
         <v>10</v>
@@ -5544,15 +5544,15 @@
         <v>51</v>
       </c>
       <c r="Q115" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="116" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
+        <v>405</v>
+      </c>
+      <c r="B116" t="s">
         <v>406</v>
-      </c>
-      <c r="B116" t="s">
-        <v>407</v>
       </c>
       <c r="C116" t="s">
         <v>10</v>
@@ -5573,16 +5573,16 @@
         <v>9</v>
       </c>
       <c r="I116" t="s">
+        <v>409</v>
+      </c>
+      <c r="J116" t="s">
         <v>410</v>
       </c>
-      <c r="J116" t="s">
-        <v>411</v>
-      </c>
       <c r="K116">
         <v>10</v>
       </c>
       <c r="Q116" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T116" t="s">
         <v>155</v>
@@ -5590,10 +5590,10 @@
     </row>
     <row r="117" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B117" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C117" t="s">
         <v>10</v>
@@ -5614,16 +5614,16 @@
         <v>9</v>
       </c>
       <c r="I117" t="s">
+        <v>413</v>
+      </c>
+      <c r="J117" t="s">
         <v>414</v>
       </c>
-      <c r="J117" t="s">
-        <v>415</v>
-      </c>
       <c r="K117">
         <v>10</v>
       </c>
       <c r="Q117" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="T117" t="s">
         <v>155</v>
@@ -5631,10 +5631,10 @@
     </row>
     <row r="118" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B118" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C118" t="s">
         <v>10</v>
@@ -5655,10 +5655,10 @@
         <v>9</v>
       </c>
       <c r="I118" t="s">
+        <v>418</v>
+      </c>
+      <c r="J118" t="s">
         <v>419</v>
-      </c>
-      <c r="J118" t="s">
-        <v>420</v>
       </c>
       <c r="K118">
         <v>10</v>
@@ -5667,15 +5667,15 @@
         <v>51</v>
       </c>
       <c r="Q118" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="119" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B119" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C119" t="s">
         <v>10</v>
@@ -5696,10 +5696,10 @@
         <v>9</v>
       </c>
       <c r="I119" t="s">
+        <v>421</v>
+      </c>
+      <c r="J119" t="s">
         <v>422</v>
-      </c>
-      <c r="J119" t="s">
-        <v>423</v>
       </c>
       <c r="K119">
         <v>5</v>
@@ -5713,10 +5713,10 @@
     </row>
     <row r="120" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B120" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C120" t="s">
         <v>10</v>
@@ -5737,24 +5737,24 @@
         <v>1</v>
       </c>
       <c r="I120" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="J120" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="K120">
         <v>10</v>
       </c>
       <c r="S120" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="121" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B121" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C121" t="s">
         <v>10</v>
@@ -5772,7 +5772,7 @@
         <v>12</v>
       </c>
       <c r="I121" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K121">
         <v>10</v>
@@ -5783,10 +5783,10 @@
     </row>
     <row r="122" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
+        <v>430</v>
+      </c>
+      <c r="B122" t="s">
         <v>431</v>
-      </c>
-      <c r="B122" t="s">
-        <v>432</v>
       </c>
       <c r="C122" t="s">
         <v>10</v>
@@ -5804,21 +5804,21 @@
         <v>9</v>
       </c>
       <c r="I122" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="K122">
         <v>10</v>
       </c>
       <c r="Q122" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="123" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B123" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C123" t="s">
         <v>10</v>
@@ -5836,7 +5836,7 @@
         <v>12</v>
       </c>
       <c r="I123" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="Q123" t="s">
         <v>162</v>
@@ -5844,10 +5844,10 @@
     </row>
     <row r="124" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
+        <v>435</v>
+      </c>
+      <c r="B124" t="s">
         <v>436</v>
-      </c>
-      <c r="B124" t="s">
-        <v>437</v>
       </c>
       <c r="C124" t="s">
         <v>10</v>
@@ -5868,15 +5868,15 @@
         <v>9</v>
       </c>
       <c r="I124" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="125" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B125" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C125" t="s">
         <v>11</v>
@@ -5897,10 +5897,10 @@
         <v>9</v>
       </c>
       <c r="I125" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="J125" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="K125">
         <v>30</v>
@@ -5911,10 +5911,10 @@
     </row>
     <row r="126" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B126" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C126" t="s">
         <v>11</v>
@@ -5935,10 +5935,10 @@
         <v>9</v>
       </c>
       <c r="I126" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="J126" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="K126">
         <v>10</v>
@@ -5949,10 +5949,10 @@
     </row>
     <row r="127" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B127" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C127" t="s">
         <v>11</v>
@@ -5973,10 +5973,10 @@
         <v>9</v>
       </c>
       <c r="I127" t="s">
+        <v>334</v>
+      </c>
+      <c r="J127" t="s">
         <v>335</v>
-      </c>
-      <c r="J127" t="s">
-        <v>336</v>
       </c>
       <c r="K127">
         <v>10</v>
@@ -5988,7 +5988,7 @@
         <v>52</v>
       </c>
       <c r="R127" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="U127" t="s">
         <v>155</v>
@@ -5996,10 +5996,10 @@
     </row>
     <row r="128" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
+        <v>441</v>
+      </c>
+      <c r="B128" t="s">
         <v>442</v>
-      </c>
-      <c r="B128" t="s">
-        <v>443</v>
       </c>
       <c r="C128" t="s">
         <v>11</v>
@@ -6020,10 +6020,10 @@
         <v>8</v>
       </c>
       <c r="I128" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="J128" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="K128">
         <v>30</v>
@@ -6037,10 +6037,10 @@
     </row>
     <row r="129" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B129" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C129" t="s">
         <v>11</v>
@@ -6061,10 +6061,10 @@
         <v>8</v>
       </c>
       <c r="I129" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J129" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="K129">
         <v>30</v>
@@ -6078,10 +6078,10 @@
     </row>
     <row r="130" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B130" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C130" t="s">
         <v>11</v>
@@ -6102,10 +6102,10 @@
         <v>8</v>
       </c>
       <c r="I130" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="J130" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="K130">
         <v>30</v>
@@ -6114,15 +6114,15 @@
         <v>51</v>
       </c>
       <c r="Q130" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="131" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B131" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C131" t="s">
         <v>11</v>
@@ -6143,10 +6143,10 @@
         <v>9</v>
       </c>
       <c r="I131" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="J131" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="K131">
         <v>30</v>
@@ -6157,10 +6157,10 @@
     </row>
     <row r="132" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
+        <v>454</v>
+      </c>
+      <c r="B132" t="s">
         <v>455</v>
-      </c>
-      <c r="B132" t="s">
-        <v>456</v>
       </c>
       <c r="C132" t="s">
         <v>11</v>
@@ -6181,10 +6181,10 @@
         <v>8</v>
       </c>
       <c r="I132" t="s">
+        <v>361</v>
+      </c>
+      <c r="J132" t="s">
         <v>362</v>
-      </c>
-      <c r="J132" t="s">
-        <v>363</v>
       </c>
       <c r="K132">
         <v>30</v>
@@ -6198,10 +6198,10 @@
     </row>
     <row r="133" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
+        <v>456</v>
+      </c>
+      <c r="B133" t="s">
         <v>457</v>
-      </c>
-      <c r="B133" t="s">
-        <v>458</v>
       </c>
       <c r="C133" t="s">
         <v>11</v>
@@ -6222,10 +6222,10 @@
         <v>13</v>
       </c>
       <c r="I133" t="s">
+        <v>458</v>
+      </c>
+      <c r="J133" t="s">
         <v>459</v>
-      </c>
-      <c r="J133" t="s">
-        <v>460</v>
       </c>
       <c r="K133">
         <v>10</v>
@@ -6239,10 +6239,10 @@
     </row>
     <row r="134" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B134" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C134" t="s">
         <v>11</v>
@@ -6263,10 +6263,10 @@
         <v>9</v>
       </c>
       <c r="I134" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J134" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="K134">
         <v>30</v>
@@ -6278,15 +6278,15 @@
         <v>52</v>
       </c>
       <c r="S134" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="135" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B135" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C135" t="s">
         <v>11</v>
@@ -6307,10 +6307,10 @@
         <v>9</v>
       </c>
       <c r="I135" t="s">
+        <v>465</v>
+      </c>
+      <c r="J135" t="s">
         <v>466</v>
-      </c>
-      <c r="J135" t="s">
-        <v>467</v>
       </c>
       <c r="K135">
         <v>10</v>
@@ -6324,10 +6324,10 @@
     </row>
     <row r="136" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
+        <v>467</v>
+      </c>
+      <c r="B136" t="s">
         <v>468</v>
-      </c>
-      <c r="B136" t="s">
-        <v>469</v>
       </c>
       <c r="C136" t="s">
         <v>11</v>
@@ -6348,10 +6348,10 @@
         <v>9</v>
       </c>
       <c r="I136" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="J136" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="K136">
         <v>10</v>
@@ -6360,15 +6360,15 @@
         <v>51</v>
       </c>
       <c r="Q136" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="137" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
+        <v>471</v>
+      </c>
+      <c r="B137" t="s">
         <v>472</v>
-      </c>
-      <c r="B137" t="s">
-        <v>473</v>
       </c>
       <c r="C137" t="s">
         <v>11</v>
@@ -6389,10 +6389,10 @@
         <v>9</v>
       </c>
       <c r="I137" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="J137" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="K137">
         <v>10</v>
@@ -6401,15 +6401,15 @@
         <v>51</v>
       </c>
       <c r="Q137" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="138" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
+        <v>475</v>
+      </c>
+      <c r="B138" t="s">
         <v>476</v>
-      </c>
-      <c r="B138" t="s">
-        <v>477</v>
       </c>
       <c r="C138" t="s">
         <v>11</v>
@@ -6430,10 +6430,10 @@
         <v>9</v>
       </c>
       <c r="I138" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="J138" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="K138">
         <v>10</v>
@@ -6444,7 +6444,7 @@
     </row>
     <row r="139" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B139" t="s">
         <v>48</v>
@@ -6468,10 +6468,10 @@
         <v>9</v>
       </c>
       <c r="I139" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="J139" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K139">
         <v>10</v>
@@ -6485,10 +6485,10 @@
     </row>
     <row r="140" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
+        <v>482</v>
+      </c>
+      <c r="B140" t="s">
         <v>483</v>
-      </c>
-      <c r="B140" t="s">
-        <v>484</v>
       </c>
       <c r="C140" t="s">
         <v>11</v>
@@ -6509,10 +6509,10 @@
         <v>9</v>
       </c>
       <c r="I140" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="J140" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="K140">
         <v>10</v>
@@ -6523,10 +6523,10 @@
     </row>
     <row r="141" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B141" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C141" t="s">
         <v>11</v>
@@ -6547,10 +6547,10 @@
         <v>9</v>
       </c>
       <c r="I141" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="J141" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="K141">
         <v>10</v>
@@ -6562,15 +6562,15 @@
         <v>104</v>
       </c>
       <c r="R141" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="142" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B142" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C142" t="s">
         <v>11</v>
@@ -6591,10 +6591,10 @@
         <v>6</v>
       </c>
       <c r="I142" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J142" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="K142">
         <v>10</v>
@@ -6605,10 +6605,10 @@
     </row>
     <row r="143" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B143" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C143" t="s">
         <v>11</v>
@@ -6629,10 +6629,10 @@
         <v>9</v>
       </c>
       <c r="I143" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="J143" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="K143">
         <v>10</v>
@@ -6641,15 +6641,15 @@
         <v>51</v>
       </c>
       <c r="Q143" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="144" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B144" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C144" t="s">
         <v>11</v>
@@ -6670,10 +6670,10 @@
         <v>9</v>
       </c>
       <c r="I144" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="J144" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="K144">
         <v>10</v>
@@ -6687,10 +6687,10 @@
     </row>
     <row r="145" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B145" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C145" t="s">
         <v>11</v>
@@ -6711,10 +6711,10 @@
         <v>9</v>
       </c>
       <c r="I145" t="s">
+        <v>503</v>
+      </c>
+      <c r="J145" t="s">
         <v>504</v>
-      </c>
-      <c r="J145" t="s">
-        <v>505</v>
       </c>
       <c r="K145">
         <v>10</v>
@@ -6728,10 +6728,10 @@
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
+        <v>505</v>
+      </c>
+      <c r="B146" t="s">
         <v>506</v>
-      </c>
-      <c r="B146" t="s">
-        <v>507</v>
       </c>
       <c r="C146" t="s">
         <v>11</v>
@@ -6752,10 +6752,10 @@
         <v>9</v>
       </c>
       <c r="I146" t="s">
+        <v>421</v>
+      </c>
+      <c r="J146" t="s">
         <v>422</v>
-      </c>
-      <c r="J146" t="s">
-        <v>423</v>
       </c>
       <c r="K146">
         <v>10</v>
@@ -6769,10 +6769,10 @@
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B147" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C147" t="s">
         <v>11</v>
@@ -6790,7 +6790,7 @@
         <v>12</v>
       </c>
       <c r="I147" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="K147">
         <v>10</v>
@@ -6801,10 +6801,10 @@
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B148" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C148" t="s">
         <v>11</v>
@@ -6822,21 +6822,21 @@
         <v>9</v>
       </c>
       <c r="I148" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="K148">
         <v>10</v>
       </c>
       <c r="Q148" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B149" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C149" t="s">
         <v>11</v>
@@ -6854,21 +6854,21 @@
         <v>12</v>
       </c>
       <c r="I149" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="K149">
         <v>10</v>
       </c>
       <c r="Q149" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B150" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C150" t="s">
         <v>11</v>
@@ -6886,18 +6886,18 @@
         <v>8</v>
       </c>
       <c r="I150" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="K150">
         <v>10</v>
       </c>
       <c r="Q150" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B151" t="s">
         <v>130</v>
@@ -6915,7 +6915,7 @@
         <v>0</v>
       </c>
       <c r="I151" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K151">
         <v>10</v>
@@ -6930,8 +6930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD92D53-EC10-4CE0-957A-62D9B9206E5C}">
   <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6946,7 +6946,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -6954,7 +6954,7 @@
     <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B3">
         <f>1024/24</f>
@@ -6963,7 +6963,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -6971,7 +6971,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B5">
         <v>8</v>
@@ -6979,7 +6979,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -8028,6 +8028,126 @@
         <v>17</v>
       </c>
     </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="str">
+        <f>Source!A86</f>
+        <v>NeutronAss</v>
+      </c>
+      <c r="B43">
+        <f>Source!C86 * Results!$B$6</f>
+        <v>9</v>
+      </c>
+      <c r="C43">
+        <f>Source!D86*Results!$B$4</f>
+        <v>32</v>
+      </c>
+      <c r="D43" s="8">
+        <f>Source!E86*Results!$B$3</f>
+        <v>1493.3333333333333</v>
+      </c>
+      <c r="E43">
+        <f>Source!H86*Results!$B$5</f>
+        <v>96</v>
+      </c>
+      <c r="F43" t="str">
+        <f>Source!F86</f>
+        <v>E3</v>
+      </c>
+      <c r="G43">
+        <f>Source!G86</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="str">
+        <f>Source!A87</f>
+        <v>Shredder</v>
+      </c>
+      <c r="B44">
+        <f>Source!C87 * Results!$B$6</f>
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <f>Source!D87*Results!$B$4</f>
+        <v>0</v>
+      </c>
+      <c r="D44" s="8">
+        <f>Source!E87*Results!$B$3</f>
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <f>Source!H87*Results!$B$5</f>
+        <v>8</v>
+      </c>
+      <c r="F44" t="str">
+        <f>Source!F87</f>
+        <v>S2</v>
+      </c>
+      <c r="G44">
+        <f>Source!G87</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="str">
+        <f>Source!A88</f>
+        <v>Contaminator</v>
+      </c>
+      <c r="B45">
+        <f>Source!C88 * Results!$B$6</f>
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <f>Source!D88*Results!$B$4</f>
+        <v>2</v>
+      </c>
+      <c r="D45" s="8">
+        <f>Source!E88*Results!$B$3</f>
+        <v>853.33333333333326</v>
+      </c>
+      <c r="E45">
+        <f>Source!H88*Results!$B$5</f>
+        <v>64</v>
+      </c>
+      <c r="F45" t="str">
+        <f>Source!F88</f>
+        <v>R2</v>
+      </c>
+      <c r="G45">
+        <f>Source!G88</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="str">
+        <f>Source!A89</f>
+        <v>LaserPistol</v>
+      </c>
+      <c r="B46">
+        <f>Source!C89 * Results!$B$6</f>
+        <v>3</v>
+      </c>
+      <c r="C46">
+        <f>Source!D89*Results!$B$4</f>
+        <v>5</v>
+      </c>
+      <c r="D46" s="8">
+        <f>Source!E89*Results!$B$3</f>
+        <v>853.33333333333326</v>
+      </c>
+      <c r="E46">
+        <f>Source!H89*Results!$B$5</f>
+        <v>64</v>
+      </c>
+      <c r="F46" t="str">
+        <f>Source!F89</f>
+        <v>E2</v>
+      </c>
+      <c r="G46">
+        <f>Source!G89</f>
+        <v>5</v>
+      </c>
+    </row>
     <row r="60" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>0</v>
@@ -8039,7 +8159,7 @@
         <v>9</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Altered movement speeds across the board to be higher. Removed 800 ticks before dying for structures. Added custom campaign map. Added rowdy civilian. Added a test buildable wall.
</commit_message>
<xml_diff>
--- a/mods/dr/The Spreadsheet.xlsx
+++ b/mods/dr/The Spreadsheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{21D69477-E333-4529-8CC7-8E3BA8C2E6F7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8D9CB213-48F0-430C-A113-BA46C527A65C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="3225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Source" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="529">
   <si>
     <t>Unit</t>
   </si>
@@ -956,12 +956,6 @@
     <t>Dark Reign Unit, Weapon, and Building values</t>
   </si>
   <si>
-    <t>Velocity Formula</t>
-  </si>
-  <si>
-    <t>Size Formula</t>
-  </si>
-  <si>
     <t>Construction Rig</t>
   </si>
   <si>
@@ -1268,9 +1262,6 @@
     <t>ufoutmn0</t>
   </si>
   <si>
-    <t>Ammo</t>
-  </si>
-  <si>
     <t>Shock Wave</t>
   </si>
   <si>
@@ -1580,18 +1571,12 @@
     <t>Converted OpenRA values</t>
   </si>
   <si>
-    <t>Time Formula</t>
-  </si>
-  <si>
     <t>Min Projectile Speed</t>
   </si>
   <si>
     <t>Max Projectile Speed</t>
   </si>
   <si>
-    <t>Cell Size formula</t>
-  </si>
-  <si>
     <t>FG AA</t>
   </si>
   <si>
@@ -1605,6 +1590,24 @@
   </si>
   <si>
     <t>FG Rail Turret</t>
+  </si>
+  <si>
+    <t>I Neutron Accelerator</t>
+  </si>
+  <si>
+    <t>Move Speed</t>
+  </si>
+  <si>
+    <t>Fire Delay Formula</t>
+  </si>
+  <si>
+    <t>Impact Radius Formula</t>
+  </si>
+  <si>
+    <t>Projectile Speed Formula</t>
+  </si>
+  <si>
+    <t>Movement Speed Formula</t>
   </si>
 </sst>
 </file>
@@ -2041,8 +2044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="B115" workbookViewId="0">
+      <selection activeCell="I146" sqref="I146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3220,10 +3223,10 @@
       </c>
       <c r="P51" s="5"/>
       <c r="U51" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="V51" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
@@ -3795,7 +3798,7 @@
         <v>150</v>
       </c>
       <c r="B67" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="C67" s="1">
         <v>20</v>
@@ -3836,7 +3839,7 @@
         <v>157</v>
       </c>
       <c r="B68" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="C68">
         <v>10</v>
@@ -3877,7 +3880,7 @@
         <v>162</v>
       </c>
       <c r="B69" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="C69">
         <v>9</v>
@@ -4000,7 +4003,7 @@
         <v>173</v>
       </c>
       <c r="B72" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="C72">
         <v>5</v>
@@ -4041,7 +4044,7 @@
         <v>289</v>
       </c>
       <c r="B73" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="C73">
         <v>5</v>
@@ -4483,6 +4486,9 @@
       <c r="A86" t="s">
         <v>225</v>
       </c>
+      <c r="B86" t="s">
+        <v>523</v>
+      </c>
       <c r="C86">
         <v>9</v>
       </c>
@@ -4694,51 +4700,51 @@
         <v>4</v>
       </c>
       <c r="G95" s="7" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="H95" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I95" s="5" t="s">
+      <c r="I95" s="7" t="s">
+        <v>524</v>
+      </c>
+      <c r="J95" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J95" s="5" t="s">
+      <c r="K95" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="L95" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="M95" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="K95" s="5" t="s">
-        <v>320</v>
-      </c>
-      <c r="L95" s="7" t="s">
-        <v>316</v>
-      </c>
-      <c r="M95" s="7" t="s">
-        <v>317</v>
-      </c>
-      <c r="O95" s="7" t="s">
-        <v>367</v>
-      </c>
-      <c r="Q95" s="7" t="s">
+      <c r="N95" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="P95" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="R95" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="S95" t="s">
-        <v>376</v>
-      </c>
       <c r="T95" t="s">
-        <v>407</v>
+        <v>374</v>
       </c>
       <c r="U95" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="V95" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
     </row>
     <row r="96" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B96" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C96" t="s">
         <v>10</v>
@@ -4758,25 +4764,28 @@
       <c r="H96">
         <v>9</v>
       </c>
-      <c r="I96" t="s">
-        <v>331</v>
+      <c r="I96">
+        <v>6</v>
       </c>
       <c r="J96" t="s">
-        <v>315</v>
-      </c>
-      <c r="K96">
+        <v>329</v>
+      </c>
+      <c r="K96" t="s">
+        <v>313</v>
+      </c>
+      <c r="L96">
         <v>30</v>
       </c>
-      <c r="O96" t="s">
+      <c r="P96" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B97" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C97" t="s">
         <v>10</v>
@@ -4796,25 +4805,28 @@
       <c r="H97">
         <v>9</v>
       </c>
-      <c r="I97" t="s">
-        <v>332</v>
+      <c r="I97">
+        <v>10</v>
       </c>
       <c r="J97" t="s">
-        <v>323</v>
-      </c>
-      <c r="K97">
-        <v>10</v>
-      </c>
-      <c r="O97" t="s">
+        <v>330</v>
+      </c>
+      <c r="K97" t="s">
+        <v>321</v>
+      </c>
+      <c r="L97">
+        <v>10</v>
+      </c>
+      <c r="P97" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B98" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C98" t="s">
         <v>10</v>
@@ -4834,34 +4846,37 @@
       <c r="H98">
         <v>9</v>
       </c>
-      <c r="I98" t="s">
-        <v>334</v>
+      <c r="I98">
+        <v>16</v>
       </c>
       <c r="J98" t="s">
+        <v>332</v>
+      </c>
+      <c r="K98" t="s">
+        <v>333</v>
+      </c>
+      <c r="L98">
+        <v>10</v>
+      </c>
+      <c r="P98" t="s">
+        <v>51</v>
+      </c>
+      <c r="R98" t="s">
+        <v>52</v>
+      </c>
+      <c r="S98" t="s">
         <v>335</v>
       </c>
-      <c r="K98">
-        <v>10</v>
-      </c>
-      <c r="O98" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q98" t="s">
-        <v>52</v>
-      </c>
-      <c r="R98" t="s">
-        <v>337</v>
-      </c>
-      <c r="U98" t="s">
+      <c r="V98" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B99" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C99" t="s">
         <v>10</v>
@@ -4881,28 +4896,31 @@
       <c r="H99">
         <v>8</v>
       </c>
-      <c r="I99" t="s">
-        <v>330</v>
+      <c r="I99">
+        <v>8</v>
       </c>
       <c r="J99" t="s">
+        <v>328</v>
+      </c>
+      <c r="K99" t="s">
+        <v>323</v>
+      </c>
+      <c r="L99">
+        <v>30</v>
+      </c>
+      <c r="P99" t="s">
+        <v>51</v>
+      </c>
+      <c r="R99" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="100" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>325</v>
       </c>
-      <c r="K99">
-        <v>30</v>
-      </c>
-      <c r="O99" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q99" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>327</v>
-      </c>
       <c r="B100" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C100" t="s">
         <v>10</v>
@@ -4922,28 +4940,31 @@
       <c r="H100">
         <v>8</v>
       </c>
-      <c r="I100" t="s">
-        <v>338</v>
+      <c r="I100">
+        <v>8</v>
       </c>
       <c r="J100" t="s">
-        <v>329</v>
-      </c>
-      <c r="K100">
+        <v>336</v>
+      </c>
+      <c r="K100" t="s">
+        <v>327</v>
+      </c>
+      <c r="L100">
         <v>30</v>
       </c>
-      <c r="O100" t="s">
+      <c r="P100" t="s">
         <v>51</v>
       </c>
-      <c r="Q100" s="1" t="s">
+      <c r="R100" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B101" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C101" t="s">
         <v>10</v>
@@ -4963,25 +4984,28 @@
       <c r="H101">
         <v>12</v>
       </c>
-      <c r="I101" t="s">
-        <v>342</v>
+      <c r="I101">
+        <v>12</v>
       </c>
       <c r="J101" t="s">
         <v>340</v>
       </c>
-      <c r="K101">
+      <c r="K101" t="s">
+        <v>338</v>
+      </c>
+      <c r="L101">
         <v>30</v>
       </c>
-      <c r="Q101" t="s">
+      <c r="R101" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B102" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C102" t="s">
         <v>10</v>
@@ -5001,22 +5025,25 @@
       <c r="H102">
         <v>12</v>
       </c>
-      <c r="I102" t="s">
+      <c r="I102">
+        <v>12</v>
+      </c>
+      <c r="J102" t="s">
+        <v>344</v>
+      </c>
+      <c r="K102" t="s">
+        <v>343</v>
+      </c>
+      <c r="L102">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="103" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>345</v>
+      </c>
+      <c r="B103" t="s">
         <v>346</v>
-      </c>
-      <c r="J102" t="s">
-        <v>345</v>
-      </c>
-      <c r="K102">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>347</v>
-      </c>
-      <c r="B103" t="s">
-        <v>348</v>
       </c>
       <c r="C103" t="s">
         <v>10</v>
@@ -5036,28 +5063,31 @@
       <c r="H103">
         <v>8</v>
       </c>
-      <c r="I103" t="s">
-        <v>350</v>
+      <c r="I103">
+        <v>8</v>
       </c>
       <c r="J103" t="s">
+        <v>348</v>
+      </c>
+      <c r="K103" t="s">
+        <v>347</v>
+      </c>
+      <c r="L103">
+        <v>30</v>
+      </c>
+      <c r="P103" t="s">
+        <v>51</v>
+      </c>
+      <c r="R103" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="104" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>349</v>
       </c>
-      <c r="K103">
-        <v>30</v>
-      </c>
-      <c r="O103" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q103" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+      <c r="B104" t="s">
         <v>351</v>
-      </c>
-      <c r="B104" t="s">
-        <v>353</v>
       </c>
       <c r="C104" t="s">
         <v>10</v>
@@ -5077,25 +5107,28 @@
       <c r="H104">
         <v>9</v>
       </c>
-      <c r="I104" t="s">
-        <v>354</v>
+      <c r="I104">
+        <v>12</v>
       </c>
       <c r="J104" t="s">
         <v>352</v>
       </c>
-      <c r="K104">
+      <c r="K104" t="s">
+        <v>350</v>
+      </c>
+      <c r="L104">
         <v>30</v>
       </c>
-      <c r="O104" t="s">
+      <c r="P104" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B105" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C105" t="s">
         <v>10</v>
@@ -5115,28 +5148,31 @@
       <c r="H105">
         <v>8</v>
       </c>
-      <c r="I105" t="s">
+      <c r="I105">
+        <v>12</v>
+      </c>
+      <c r="J105" t="s">
+        <v>356</v>
+      </c>
+      <c r="K105" t="s">
+        <v>355</v>
+      </c>
+      <c r="L105">
+        <v>30</v>
+      </c>
+      <c r="P105" t="s">
+        <v>51</v>
+      </c>
+      <c r="R105" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="106" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>358</v>
       </c>
-      <c r="J105" t="s">
+      <c r="B106" t="s">
         <v>357</v>
-      </c>
-      <c r="K105">
-        <v>30</v>
-      </c>
-      <c r="O105" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q105" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>360</v>
-      </c>
-      <c r="B106" t="s">
-        <v>359</v>
       </c>
       <c r="C106" t="s">
         <v>10</v>
@@ -5156,25 +5192,28 @@
       <c r="H106">
         <v>8</v>
       </c>
-      <c r="I106" t="s">
+      <c r="I106">
+        <v>16</v>
+      </c>
+      <c r="J106" t="s">
+        <v>359</v>
+      </c>
+      <c r="K106" t="s">
+        <v>360</v>
+      </c>
+      <c r="L106">
+        <v>30</v>
+      </c>
+      <c r="R106" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="107" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>362</v>
+      </c>
+      <c r="B107" t="s">
         <v>361</v>
-      </c>
-      <c r="J106" t="s">
-        <v>362</v>
-      </c>
-      <c r="K106">
-        <v>30</v>
-      </c>
-      <c r="Q106" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="107" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>364</v>
-      </c>
-      <c r="B107" t="s">
-        <v>363</v>
       </c>
       <c r="D107">
         <v>1000</v>
@@ -5191,25 +5230,28 @@
       <c r="H107">
         <v>9</v>
       </c>
-      <c r="I107" t="s">
+      <c r="I107">
+        <v>12</v>
+      </c>
+      <c r="J107" t="s">
+        <v>364</v>
+      </c>
+      <c r="K107" t="s">
+        <v>363</v>
+      </c>
+      <c r="L107">
+        <v>30</v>
+      </c>
+      <c r="P107" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="108" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>366</v>
       </c>
-      <c r="J107" t="s">
-        <v>365</v>
-      </c>
-      <c r="K107">
-        <v>30</v>
-      </c>
-      <c r="O107" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="108" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>368</v>
-      </c>
       <c r="B108" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C108" t="s">
         <v>10</v>
@@ -5229,28 +5271,31 @@
       <c r="H108">
         <v>9</v>
       </c>
-      <c r="I108" t="s">
+      <c r="I108">
+        <v>24</v>
+      </c>
+      <c r="J108" t="s">
+        <v>369</v>
+      </c>
+      <c r="K108" t="s">
+        <v>368</v>
+      </c>
+      <c r="L108">
+        <v>10</v>
+      </c>
+      <c r="P108" t="s">
+        <v>51</v>
+      </c>
+      <c r="R108" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="109" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>371</v>
       </c>
-      <c r="J108" t="s">
+      <c r="B109" t="s">
         <v>370</v>
-      </c>
-      <c r="K108">
-        <v>10</v>
-      </c>
-      <c r="O108" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q108" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="109" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>373</v>
-      </c>
-      <c r="B109" t="s">
-        <v>372</v>
       </c>
       <c r="C109" t="s">
         <v>10</v>
@@ -5270,31 +5315,34 @@
       <c r="H109">
         <v>9</v>
       </c>
-      <c r="I109" t="s">
+      <c r="I109">
+        <v>18</v>
+      </c>
+      <c r="J109" t="s">
+        <v>373</v>
+      </c>
+      <c r="K109" t="s">
+        <v>372</v>
+      </c>
+      <c r="L109">
+        <v>12</v>
+      </c>
+      <c r="P109" t="s">
+        <v>51</v>
+      </c>
+      <c r="T109" t="s">
         <v>375</v>
       </c>
-      <c r="J109" t="s">
-        <v>374</v>
-      </c>
-      <c r="K109">
-        <v>12</v>
-      </c>
-      <c r="O109" t="s">
-        <v>51</v>
-      </c>
-      <c r="S109" t="s">
-        <v>377</v>
-      </c>
-      <c r="U109" t="s">
+      <c r="V109" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="110" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B110" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C110" t="s">
         <v>10</v>
@@ -5314,34 +5362,37 @@
       <c r="H110">
         <v>9</v>
       </c>
-      <c r="I110" t="s">
+      <c r="I110">
+        <v>16</v>
+      </c>
+      <c r="J110" t="s">
+        <v>378</v>
+      </c>
+      <c r="K110" t="s">
+        <v>377</v>
+      </c>
+      <c r="L110">
+        <v>10</v>
+      </c>
+      <c r="P110" t="s">
+        <v>51</v>
+      </c>
+      <c r="R110" t="s">
+        <v>80</v>
+      </c>
+      <c r="U110" t="s">
+        <v>379</v>
+      </c>
+      <c r="V110" t="s">
         <v>380</v>
       </c>
-      <c r="J110" t="s">
-        <v>379</v>
-      </c>
-      <c r="K110">
-        <v>10</v>
-      </c>
-      <c r="O110" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q110" t="s">
-        <v>80</v>
-      </c>
-      <c r="T110" t="s">
-        <v>381</v>
-      </c>
-      <c r="U110" t="s">
+    </row>
+    <row r="111" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>383</v>
+      </c>
+      <c r="B111" t="s">
         <v>382</v>
-      </c>
-    </row>
-    <row r="111" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>385</v>
-      </c>
-      <c r="B111" t="s">
-        <v>384</v>
       </c>
       <c r="C111" t="s">
         <v>10</v>
@@ -5361,28 +5412,31 @@
       <c r="H111">
         <v>9</v>
       </c>
-      <c r="I111" t="s">
+      <c r="I111">
+        <v>20</v>
+      </c>
+      <c r="J111" t="s">
+        <v>385</v>
+      </c>
+      <c r="K111" t="s">
+        <v>384</v>
+      </c>
+      <c r="L111">
+        <v>30</v>
+      </c>
+      <c r="P111" t="s">
+        <v>51</v>
+      </c>
+      <c r="R111" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="112" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>387</v>
       </c>
-      <c r="J111" t="s">
+      <c r="B112" t="s">
         <v>386</v>
-      </c>
-      <c r="K111">
-        <v>30</v>
-      </c>
-      <c r="O111" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q111" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="112" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>389</v>
-      </c>
-      <c r="B112" t="s">
-        <v>388</v>
       </c>
       <c r="C112" t="s">
         <v>10</v>
@@ -5402,28 +5456,31 @@
       <c r="H112">
         <v>9</v>
       </c>
-      <c r="I112" t="s">
-        <v>394</v>
+      <c r="I112">
+        <v>12</v>
       </c>
       <c r="J112" t="s">
+        <v>392</v>
+      </c>
+      <c r="K112" t="s">
+        <v>388</v>
+      </c>
+      <c r="L112">
+        <v>10</v>
+      </c>
+      <c r="P112" t="s">
+        <v>51</v>
+      </c>
+      <c r="R112" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="113" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>390</v>
       </c>
-      <c r="K112">
-        <v>10</v>
-      </c>
-      <c r="O112" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q112" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="113" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>392</v>
-      </c>
       <c r="B113" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C113" t="s">
         <v>10</v>
@@ -5443,28 +5500,31 @@
       <c r="H113">
         <v>9</v>
       </c>
-      <c r="I113" t="s">
-        <v>395</v>
+      <c r="I113">
+        <v>12</v>
       </c>
       <c r="J113" t="s">
         <v>393</v>
       </c>
-      <c r="K113">
+      <c r="K113" t="s">
+        <v>391</v>
+      </c>
+      <c r="L113">
         <v>30</v>
       </c>
-      <c r="O113" t="s">
+      <c r="P113" t="s">
         <v>51</v>
       </c>
-      <c r="Q113" t="s">
+      <c r="R113" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="114" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B114" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C114" t="s">
         <v>10</v>
@@ -5484,34 +5544,37 @@
       <c r="H114">
         <v>9</v>
       </c>
-      <c r="I114" t="s">
+      <c r="I114">
+        <v>12</v>
+      </c>
+      <c r="J114" t="s">
+        <v>396</v>
+      </c>
+      <c r="K114" t="s">
         <v>398</v>
       </c>
-      <c r="J114" t="s">
+      <c r="L114">
+        <v>10</v>
+      </c>
+      <c r="P114" t="s">
+        <v>51</v>
+      </c>
+      <c r="R114" t="s">
+        <v>75</v>
+      </c>
+      <c r="U114" t="s">
+        <v>397</v>
+      </c>
+      <c r="V114" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="115" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>399</v>
+      </c>
+      <c r="B115" t="s">
         <v>400</v>
-      </c>
-      <c r="K114">
-        <v>10</v>
-      </c>
-      <c r="O114" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q114" t="s">
-        <v>75</v>
-      </c>
-      <c r="T114" t="s">
-        <v>399</v>
-      </c>
-      <c r="U114" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="115" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>401</v>
-      </c>
-      <c r="B115" t="s">
-        <v>402</v>
       </c>
       <c r="C115" t="s">
         <v>10</v>
@@ -5531,28 +5594,31 @@
       <c r="H115">
         <v>9</v>
       </c>
-      <c r="I115" t="s">
+      <c r="I115">
+        <v>8</v>
+      </c>
+      <c r="J115" t="s">
+        <v>401</v>
+      </c>
+      <c r="K115" t="s">
+        <v>402</v>
+      </c>
+      <c r="L115">
+        <v>10</v>
+      </c>
+      <c r="P115" t="s">
+        <v>51</v>
+      </c>
+      <c r="R115" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="116" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>403</v>
       </c>
-      <c r="J115" t="s">
+      <c r="B116" t="s">
         <v>404</v>
-      </c>
-      <c r="K115">
-        <v>10</v>
-      </c>
-      <c r="O115" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q115" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="116" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>405</v>
-      </c>
-      <c r="B116" t="s">
-        <v>406</v>
       </c>
       <c r="C116" t="s">
         <v>10</v>
@@ -5572,28 +5638,31 @@
       <c r="H116">
         <v>9</v>
       </c>
-      <c r="I116" t="s">
+      <c r="I116">
+        <v>28</v>
+      </c>
+      <c r="J116" t="s">
+        <v>407</v>
+      </c>
+      <c r="K116" t="s">
+        <v>408</v>
+      </c>
+      <c r="L116">
+        <v>10</v>
+      </c>
+      <c r="R116" t="s">
+        <v>168</v>
+      </c>
+      <c r="U116" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="117" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>410</v>
+      </c>
+      <c r="B117" t="s">
         <v>409</v>
-      </c>
-      <c r="J116" t="s">
-        <v>410</v>
-      </c>
-      <c r="K116">
-        <v>10</v>
-      </c>
-      <c r="Q116" t="s">
-        <v>168</v>
-      </c>
-      <c r="T116" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="117" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>412</v>
-      </c>
-      <c r="B117" t="s">
-        <v>411</v>
       </c>
       <c r="C117" t="s">
         <v>10</v>
@@ -5613,28 +5682,31 @@
       <c r="H117">
         <v>9</v>
       </c>
-      <c r="I117" t="s">
+      <c r="I117">
+        <v>24</v>
+      </c>
+      <c r="J117" t="s">
+        <v>411</v>
+      </c>
+      <c r="K117" t="s">
+        <v>412</v>
+      </c>
+      <c r="L117">
+        <v>10</v>
+      </c>
+      <c r="R117" t="s">
+        <v>188</v>
+      </c>
+      <c r="U117" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="118" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>414</v>
+      </c>
+      <c r="B118" t="s">
         <v>413</v>
-      </c>
-      <c r="J117" t="s">
-        <v>414</v>
-      </c>
-      <c r="K117">
-        <v>10</v>
-      </c>
-      <c r="Q117" t="s">
-        <v>188</v>
-      </c>
-      <c r="T117" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="118" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>417</v>
-      </c>
-      <c r="B118" t="s">
-        <v>416</v>
       </c>
       <c r="C118" t="s">
         <v>10</v>
@@ -5654,28 +5726,31 @@
       <c r="H118">
         <v>9</v>
       </c>
-      <c r="I118" t="s">
-        <v>418</v>
+      <c r="I118">
+        <v>8</v>
       </c>
       <c r="J118" t="s">
-        <v>419</v>
-      </c>
-      <c r="K118">
-        <v>10</v>
-      </c>
-      <c r="O118" t="s">
+        <v>415</v>
+      </c>
+      <c r="K118" t="s">
+        <v>416</v>
+      </c>
+      <c r="L118">
+        <v>10</v>
+      </c>
+      <c r="P118" t="s">
         <v>51</v>
       </c>
-      <c r="Q118" t="s">
+      <c r="R118" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="119" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B119" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C119" t="s">
         <v>10</v>
@@ -5695,28 +5770,31 @@
       <c r="H119">
         <v>9</v>
       </c>
-      <c r="I119" t="s">
+      <c r="I119">
+        <v>4</v>
+      </c>
+      <c r="J119" t="s">
+        <v>418</v>
+      </c>
+      <c r="K119" t="s">
+        <v>419</v>
+      </c>
+      <c r="L119">
+        <v>5</v>
+      </c>
+      <c r="P119" t="s">
+        <v>51</v>
+      </c>
+      <c r="R119" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="120" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>421</v>
       </c>
-      <c r="J119" t="s">
-        <v>422</v>
-      </c>
-      <c r="K119">
-        <v>5</v>
-      </c>
-      <c r="O119" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q119" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="120" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>424</v>
-      </c>
       <c r="B120" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C120" t="s">
         <v>10</v>
@@ -5736,25 +5814,28 @@
       <c r="H120">
         <v>1</v>
       </c>
-      <c r="I120" t="s">
-        <v>426</v>
+      <c r="I120">
+        <v>8</v>
       </c>
       <c r="J120" t="s">
-        <v>335</v>
-      </c>
-      <c r="K120">
-        <v>10</v>
-      </c>
-      <c r="S120" t="s">
+        <v>423</v>
+      </c>
+      <c r="K120" t="s">
+        <v>333</v>
+      </c>
+      <c r="L120">
+        <v>10</v>
+      </c>
+      <c r="T120" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="121" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="121" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>428</v>
-      </c>
       <c r="B121" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="C121" t="s">
         <v>10</v>
@@ -5771,22 +5852,22 @@
       <c r="H121">
         <v>12</v>
       </c>
-      <c r="I121" t="s">
-        <v>429</v>
-      </c>
-      <c r="K121">
-        <v>10</v>
-      </c>
-      <c r="Q121" t="s">
+      <c r="J121" t="s">
+        <v>426</v>
+      </c>
+      <c r="L121">
+        <v>10</v>
+      </c>
+      <c r="R121" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="122" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B122" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C122" t="s">
         <v>10</v>
@@ -5803,22 +5884,22 @@
       <c r="H122">
         <v>9</v>
       </c>
-      <c r="I122" t="s">
-        <v>432</v>
-      </c>
-      <c r="K122">
-        <v>10</v>
-      </c>
-      <c r="Q122" t="s">
+      <c r="J122" t="s">
+        <v>429</v>
+      </c>
+      <c r="L122">
+        <v>10</v>
+      </c>
+      <c r="R122" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="123" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>248</v>
       </c>
       <c r="B123" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C123" t="s">
         <v>10</v>
@@ -5835,19 +5916,19 @@
       <c r="H123">
         <v>12</v>
       </c>
-      <c r="I123" t="s">
-        <v>434</v>
-      </c>
-      <c r="Q123" t="s">
+      <c r="J123" t="s">
+        <v>431</v>
+      </c>
+      <c r="R123" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="124" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B124" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C124" t="s">
         <v>10</v>
@@ -5867,16 +5948,16 @@
       <c r="H124">
         <v>9</v>
       </c>
-      <c r="I124" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="125" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="J124" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="125" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B125" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C125" t="s">
         <v>11</v>
@@ -5896,25 +5977,28 @@
       <c r="H125">
         <v>9</v>
       </c>
-      <c r="I125" t="s">
-        <v>331</v>
+      <c r="I125">
+        <v>6</v>
       </c>
       <c r="J125" t="s">
-        <v>315</v>
-      </c>
-      <c r="K125">
+        <v>329</v>
+      </c>
+      <c r="K125" t="s">
+        <v>313</v>
+      </c>
+      <c r="L125">
         <v>30</v>
       </c>
-      <c r="O125" t="s">
+      <c r="P125" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="126" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B126" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C126" t="s">
         <v>11</v>
@@ -5934,25 +6018,28 @@
       <c r="H126">
         <v>9</v>
       </c>
-      <c r="I126" t="s">
-        <v>332</v>
+      <c r="I126">
+        <v>10</v>
       </c>
       <c r="J126" t="s">
-        <v>323</v>
-      </c>
-      <c r="K126">
-        <v>10</v>
-      </c>
-      <c r="O126" t="s">
+        <v>330</v>
+      </c>
+      <c r="K126" t="s">
+        <v>321</v>
+      </c>
+      <c r="L126">
+        <v>10</v>
+      </c>
+      <c r="P126" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="127" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="B127" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C127" t="s">
         <v>11</v>
@@ -5972,34 +6059,37 @@
       <c r="H127">
         <v>9</v>
       </c>
-      <c r="I127" t="s">
-        <v>334</v>
+      <c r="I127">
+        <v>16</v>
       </c>
       <c r="J127" t="s">
+        <v>332</v>
+      </c>
+      <c r="K127" t="s">
+        <v>333</v>
+      </c>
+      <c r="L127">
+        <v>10</v>
+      </c>
+      <c r="P127" t="s">
+        <v>51</v>
+      </c>
+      <c r="R127" t="s">
+        <v>52</v>
+      </c>
+      <c r="S127" t="s">
         <v>335</v>
       </c>
-      <c r="K127">
-        <v>10</v>
-      </c>
-      <c r="O127" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q127" t="s">
-        <v>52</v>
-      </c>
-      <c r="R127" t="s">
-        <v>337</v>
-      </c>
-      <c r="U127" t="s">
+      <c r="V127" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="128" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="B128" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C128" t="s">
         <v>11</v>
@@ -6019,28 +6109,31 @@
       <c r="H128">
         <v>8</v>
       </c>
-      <c r="I128" t="s">
-        <v>444</v>
+      <c r="I128">
+        <v>8</v>
       </c>
       <c r="J128" t="s">
+        <v>441</v>
+      </c>
+      <c r="K128" t="s">
+        <v>440</v>
+      </c>
+      <c r="L128">
+        <v>30</v>
+      </c>
+      <c r="P128" t="s">
+        <v>51</v>
+      </c>
+      <c r="R128" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
         <v>443</v>
       </c>
-      <c r="K128">
-        <v>30</v>
-      </c>
-      <c r="O128" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q128" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>446</v>
-      </c>
       <c r="B129" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C129" t="s">
         <v>11</v>
@@ -6060,28 +6153,31 @@
       <c r="H129">
         <v>8</v>
       </c>
-      <c r="I129" t="s">
-        <v>448</v>
+      <c r="I129">
+        <v>6</v>
       </c>
       <c r="J129" t="s">
+        <v>445</v>
+      </c>
+      <c r="K129" t="s">
+        <v>444</v>
+      </c>
+      <c r="L129">
+        <v>30</v>
+      </c>
+      <c r="P129" t="s">
+        <v>51</v>
+      </c>
+      <c r="R129" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="130" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>447</v>
       </c>
-      <c r="K129">
-        <v>30</v>
-      </c>
-      <c r="O129" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q129" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>450</v>
-      </c>
       <c r="B130" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="C130" t="s">
         <v>11</v>
@@ -6101,28 +6197,31 @@
       <c r="H130">
         <v>8</v>
       </c>
-      <c r="I130" t="s">
-        <v>452</v>
+      <c r="I130">
+        <v>16</v>
       </c>
       <c r="J130" t="s">
-        <v>451</v>
-      </c>
-      <c r="K130">
+        <v>449</v>
+      </c>
+      <c r="K130" t="s">
+        <v>448</v>
+      </c>
+      <c r="L130">
         <v>30</v>
       </c>
-      <c r="O130" t="s">
+      <c r="P130" t="s">
         <v>51</v>
       </c>
-      <c r="Q130" t="s">
+      <c r="R130" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="B131" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C131" t="s">
         <v>11</v>
@@ -6142,25 +6241,28 @@
       <c r="H131">
         <v>9</v>
       </c>
-      <c r="I131" t="s">
-        <v>366</v>
+      <c r="I131">
+        <v>12</v>
       </c>
       <c r="J131" t="s">
-        <v>365</v>
-      </c>
-      <c r="K131">
+        <v>364</v>
+      </c>
+      <c r="K131" t="s">
+        <v>363</v>
+      </c>
+      <c r="L131">
         <v>30</v>
       </c>
-      <c r="O131" t="s">
+      <c r="P131" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="B132" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="C132" t="s">
         <v>11</v>
@@ -6180,28 +6282,31 @@
       <c r="H132">
         <v>8</v>
       </c>
-      <c r="I132" t="s">
-        <v>361</v>
+      <c r="I132">
+        <v>6</v>
       </c>
       <c r="J132" t="s">
-        <v>362</v>
-      </c>
-      <c r="K132">
+        <v>359</v>
+      </c>
+      <c r="K132" t="s">
+        <v>360</v>
+      </c>
+      <c r="L132">
         <v>30</v>
       </c>
-      <c r="O132" t="s">
+      <c r="P132" t="s">
         <v>51</v>
       </c>
-      <c r="Q132" t="s">
+      <c r="R132" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="B133" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="C133" t="s">
         <v>11</v>
@@ -6221,28 +6326,31 @@
       <c r="H133">
         <v>13</v>
       </c>
-      <c r="I133" t="s">
+      <c r="I133">
+        <v>20</v>
+      </c>
+      <c r="J133" t="s">
+        <v>455</v>
+      </c>
+      <c r="K133" t="s">
+        <v>456</v>
+      </c>
+      <c r="L133">
+        <v>10</v>
+      </c>
+      <c r="P133" t="s">
+        <v>51</v>
+      </c>
+      <c r="R133" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="134" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
         <v>458</v>
       </c>
-      <c r="J133" t="s">
-        <v>459</v>
-      </c>
-      <c r="K133">
-        <v>10</v>
-      </c>
-      <c r="O133" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q133" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>461</v>
-      </c>
       <c r="B134" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="C134" t="s">
         <v>11</v>
@@ -6262,31 +6370,34 @@
       <c r="H134">
         <v>9</v>
       </c>
-      <c r="I134" t="s">
-        <v>337</v>
+      <c r="I134">
+        <v>20</v>
       </c>
       <c r="J134" t="s">
-        <v>462</v>
-      </c>
-      <c r="K134">
+        <v>335</v>
+      </c>
+      <c r="K134" t="s">
+        <v>459</v>
+      </c>
+      <c r="L134">
         <v>30</v>
       </c>
-      <c r="O134" t="s">
+      <c r="P134" t="s">
         <v>51</v>
       </c>
-      <c r="Q134" t="s">
+      <c r="R134" t="s">
         <v>52</v>
       </c>
-      <c r="S134" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T134" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="135" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="B135" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="C135" t="s">
         <v>11</v>
@@ -6306,28 +6417,31 @@
       <c r="H135">
         <v>9</v>
       </c>
-      <c r="I135" t="s">
+      <c r="I135">
+        <v>16</v>
+      </c>
+      <c r="J135" t="s">
+        <v>462</v>
+      </c>
+      <c r="K135" t="s">
+        <v>463</v>
+      </c>
+      <c r="L135">
+        <v>10</v>
+      </c>
+      <c r="P135" t="s">
+        <v>51</v>
+      </c>
+      <c r="R135" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="136" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>464</v>
+      </c>
+      <c r="B136" t="s">
         <v>465</v>
-      </c>
-      <c r="J135" t="s">
-        <v>466</v>
-      </c>
-      <c r="K135">
-        <v>10</v>
-      </c>
-      <c r="O135" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q135" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>467</v>
-      </c>
-      <c r="B136" t="s">
-        <v>468</v>
       </c>
       <c r="C136" t="s">
         <v>11</v>
@@ -6347,28 +6461,31 @@
       <c r="H136">
         <v>9</v>
       </c>
-      <c r="I136" t="s">
-        <v>470</v>
+      <c r="I136">
+        <v>8</v>
       </c>
       <c r="J136" t="s">
+        <v>467</v>
+      </c>
+      <c r="K136" t="s">
+        <v>466</v>
+      </c>
+      <c r="L136">
+        <v>10</v>
+      </c>
+      <c r="P136" t="s">
+        <v>51</v>
+      </c>
+      <c r="R136" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="137" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>468</v>
+      </c>
+      <c r="B137" t="s">
         <v>469</v>
-      </c>
-      <c r="K136">
-        <v>10</v>
-      </c>
-      <c r="O136" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q136" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>471</v>
-      </c>
-      <c r="B137" t="s">
-        <v>472</v>
       </c>
       <c r="C137" t="s">
         <v>11</v>
@@ -6388,28 +6505,31 @@
       <c r="H137">
         <v>9</v>
       </c>
-      <c r="I137" t="s">
-        <v>474</v>
+      <c r="I137">
+        <v>16</v>
       </c>
       <c r="J137" t="s">
+        <v>471</v>
+      </c>
+      <c r="K137" t="s">
+        <v>470</v>
+      </c>
+      <c r="L137">
+        <v>10</v>
+      </c>
+      <c r="P137" t="s">
+        <v>51</v>
+      </c>
+      <c r="R137" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="138" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>472</v>
+      </c>
+      <c r="B138" t="s">
         <v>473</v>
-      </c>
-      <c r="K137">
-        <v>10</v>
-      </c>
-      <c r="O137" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q137" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>475</v>
-      </c>
-      <c r="B138" t="s">
-        <v>476</v>
       </c>
       <c r="C138" t="s">
         <v>11</v>
@@ -6429,22 +6549,25 @@
       <c r="H138">
         <v>9</v>
       </c>
-      <c r="I138" t="s">
-        <v>478</v>
+      <c r="I138">
+        <v>16</v>
       </c>
       <c r="J138" t="s">
-        <v>477</v>
-      </c>
-      <c r="K138">
-        <v>10</v>
-      </c>
-      <c r="O138" t="s">
+        <v>475</v>
+      </c>
+      <c r="K138" t="s">
+        <v>474</v>
+      </c>
+      <c r="L138">
+        <v>10</v>
+      </c>
+      <c r="P138" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="B139" t="s">
         <v>48</v>
@@ -6467,28 +6590,31 @@
       <c r="H139">
         <v>9</v>
       </c>
-      <c r="I139" t="s">
-        <v>481</v>
+      <c r="I139">
+        <v>20</v>
       </c>
       <c r="J139" t="s">
+        <v>478</v>
+      </c>
+      <c r="K139" t="s">
+        <v>477</v>
+      </c>
+      <c r="L139">
+        <v>10</v>
+      </c>
+      <c r="P139" t="s">
+        <v>51</v>
+      </c>
+      <c r="R139" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="140" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>479</v>
+      </c>
+      <c r="B140" t="s">
         <v>480</v>
-      </c>
-      <c r="K139">
-        <v>10</v>
-      </c>
-      <c r="O139" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q139" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>482</v>
-      </c>
-      <c r="B140" t="s">
-        <v>483</v>
       </c>
       <c r="C140" t="s">
         <v>11</v>
@@ -6508,25 +6634,28 @@
       <c r="H140">
         <v>9</v>
       </c>
-      <c r="I140" t="s">
-        <v>485</v>
+      <c r="I140">
+        <v>20</v>
       </c>
       <c r="J140" t="s">
+        <v>482</v>
+      </c>
+      <c r="K140" t="s">
+        <v>481</v>
+      </c>
+      <c r="L140">
+        <v>10</v>
+      </c>
+      <c r="P140" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="141" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
         <v>484</v>
       </c>
-      <c r="K140">
-        <v>10</v>
-      </c>
-      <c r="O140" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>487</v>
-      </c>
       <c r="B141" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C141" t="s">
         <v>11</v>
@@ -6546,31 +6675,34 @@
       <c r="H141">
         <v>9</v>
       </c>
-      <c r="I141" t="s">
-        <v>489</v>
+      <c r="I141">
+        <v>12</v>
       </c>
       <c r="J141" t="s">
+        <v>486</v>
+      </c>
+      <c r="K141" t="s">
+        <v>485</v>
+      </c>
+      <c r="L141">
+        <v>10</v>
+      </c>
+      <c r="P141" t="s">
+        <v>51</v>
+      </c>
+      <c r="R141" t="s">
+        <v>104</v>
+      </c>
+      <c r="S141" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="142" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
         <v>488</v>
       </c>
-      <c r="K141">
-        <v>10</v>
-      </c>
-      <c r="O141" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q141" t="s">
-        <v>104</v>
-      </c>
-      <c r="R141" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="142" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
+      <c r="B142" t="s">
         <v>491</v>
-      </c>
-      <c r="B142" t="s">
-        <v>494</v>
       </c>
       <c r="C142" t="s">
         <v>11</v>
@@ -6590,25 +6722,28 @@
       <c r="H142">
         <v>6</v>
       </c>
-      <c r="I142" t="s">
-        <v>493</v>
+      <c r="I142">
+        <v>12</v>
       </c>
       <c r="J142" t="s">
+        <v>490</v>
+      </c>
+      <c r="K142" t="s">
+        <v>489</v>
+      </c>
+      <c r="L142">
+        <v>10</v>
+      </c>
+      <c r="P142" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="143" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
         <v>492</v>
       </c>
-      <c r="K142">
-        <v>10</v>
-      </c>
-      <c r="O142" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="143" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>495</v>
-      </c>
       <c r="B143" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="C143" t="s">
         <v>11</v>
@@ -6628,28 +6763,31 @@
       <c r="H143">
         <v>9</v>
       </c>
-      <c r="I143" t="s">
-        <v>496</v>
+      <c r="I143">
+        <v>6</v>
       </c>
       <c r="J143" t="s">
-        <v>492</v>
-      </c>
-      <c r="K143">
-        <v>10</v>
-      </c>
-      <c r="O143" t="s">
+        <v>493</v>
+      </c>
+      <c r="K143" t="s">
+        <v>489</v>
+      </c>
+      <c r="L143">
+        <v>10</v>
+      </c>
+      <c r="P143" t="s">
         <v>51</v>
       </c>
-      <c r="Q143" t="s">
+      <c r="R143" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="144" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B144" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="C144" t="s">
         <v>11</v>
@@ -6669,28 +6807,31 @@
       <c r="H144">
         <v>9</v>
       </c>
-      <c r="I144" t="s">
-        <v>500</v>
+      <c r="I144">
+        <v>24</v>
       </c>
       <c r="J144" t="s">
+        <v>497</v>
+      </c>
+      <c r="K144" t="s">
+        <v>496</v>
+      </c>
+      <c r="L144">
+        <v>10</v>
+      </c>
+      <c r="P144" t="s">
+        <v>51</v>
+      </c>
+      <c r="R144" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
         <v>499</v>
       </c>
-      <c r="K144">
-        <v>10</v>
-      </c>
-      <c r="O144" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q144" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>502</v>
-      </c>
       <c r="B145" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="C145" t="s">
         <v>11</v>
@@ -6710,28 +6851,31 @@
       <c r="H145">
         <v>9</v>
       </c>
-      <c r="I145" t="s">
+      <c r="I145">
+        <v>10</v>
+      </c>
+      <c r="J145" t="s">
+        <v>500</v>
+      </c>
+      <c r="K145" t="s">
+        <v>501</v>
+      </c>
+      <c r="L145">
+        <v>10</v>
+      </c>
+      <c r="P145" t="s">
+        <v>51</v>
+      </c>
+      <c r="R145" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>502</v>
+      </c>
+      <c r="B146" t="s">
         <v>503</v>
-      </c>
-      <c r="J145" t="s">
-        <v>504</v>
-      </c>
-      <c r="K145">
-        <v>10</v>
-      </c>
-      <c r="O145" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q145" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>505</v>
-      </c>
-      <c r="B146" t="s">
-        <v>506</v>
       </c>
       <c r="C146" t="s">
         <v>11</v>
@@ -6751,28 +6895,31 @@
       <c r="H146">
         <v>9</v>
       </c>
-      <c r="I146" t="s">
-        <v>421</v>
+      <c r="I146">
+        <v>4</v>
       </c>
       <c r="J146" t="s">
-        <v>422</v>
-      </c>
-      <c r="K146">
-        <v>10</v>
-      </c>
-      <c r="O146" t="s">
+        <v>418</v>
+      </c>
+      <c r="K146" t="s">
+        <v>419</v>
+      </c>
+      <c r="L146">
+        <v>10</v>
+      </c>
+      <c r="P146" t="s">
         <v>51</v>
       </c>
-      <c r="Q146" t="s">
+      <c r="R146" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="B147" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="C147" t="s">
         <v>11</v>
@@ -6789,22 +6936,22 @@
       <c r="H147">
         <v>12</v>
       </c>
-      <c r="I147" t="s">
-        <v>508</v>
-      </c>
-      <c r="K147">
-        <v>10</v>
-      </c>
-      <c r="Q147" t="s">
+      <c r="J147" t="s">
+        <v>505</v>
+      </c>
+      <c r="L147">
+        <v>10</v>
+      </c>
+      <c r="R147" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="B148" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C148" t="s">
         <v>11</v>
@@ -6821,22 +6968,22 @@
       <c r="H148">
         <v>9</v>
       </c>
-      <c r="I148" t="s">
-        <v>510</v>
-      </c>
-      <c r="K148">
-        <v>10</v>
-      </c>
-      <c r="Q148" t="s">
+      <c r="J148" t="s">
+        <v>507</v>
+      </c>
+      <c r="L148">
+        <v>10</v>
+      </c>
+      <c r="R148" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="B149" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C149" t="s">
         <v>11</v>
@@ -6853,22 +7000,22 @@
       <c r="H149">
         <v>12</v>
       </c>
-      <c r="I149" t="s">
-        <v>512</v>
-      </c>
-      <c r="K149">
-        <v>10</v>
-      </c>
-      <c r="Q149" t="s">
+      <c r="J149" t="s">
+        <v>509</v>
+      </c>
+      <c r="L149">
+        <v>10</v>
+      </c>
+      <c r="R149" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="B150" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="C150" t="s">
         <v>11</v>
@@ -6885,19 +7032,19 @@
       <c r="H150">
         <v>8</v>
       </c>
-      <c r="I150" t="s">
-        <v>515</v>
-      </c>
-      <c r="K150">
-        <v>10</v>
-      </c>
-      <c r="Q150" t="s">
+      <c r="J150" t="s">
+        <v>512</v>
+      </c>
+      <c r="L150">
+        <v>10</v>
+      </c>
+      <c r="R150" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="B151" t="s">
         <v>130</v>
@@ -6914,10 +7061,10 @@
       <c r="H151">
         <v>0</v>
       </c>
-      <c r="I151" t="s">
-        <v>517</v>
-      </c>
-      <c r="K151">
+      <c r="J151" t="s">
+        <v>514</v>
+      </c>
+      <c r="L151">
         <v>10</v>
       </c>
     </row>
@@ -6930,8 +7077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD92D53-EC10-4CE0-957A-62D9B9206E5C}">
   <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6946,7 +7093,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -6954,7 +7101,7 @@
     <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>311</v>
+        <v>527</v>
       </c>
       <c r="B3">
         <f>1024/24</f>
@@ -6963,7 +7110,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>519</v>
+        <v>525</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -6971,7 +7118,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>312</v>
+        <v>526</v>
       </c>
       <c r="B5">
         <v>8</v>
@@ -6979,10 +7126,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>522</v>
+        <v>528</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7014,7 +7161,7 @@
         <v>Chaff</v>
       </c>
       <c r="B9">
-        <f>Source!C52 * Results!$B$6</f>
+        <f>Source!C52</f>
         <v>8</v>
       </c>
       <c r="C9">
@@ -7044,7 +7191,7 @@
         <v>LaserRifle</v>
       </c>
       <c r="B10">
-        <f>Source!C53 * Results!$B$6</f>
+        <f>Source!C53</f>
         <v>4</v>
       </c>
       <c r="C10">
@@ -7074,7 +7221,7 @@
         <v>RailGun</v>
       </c>
       <c r="B11">
-        <f>Source!C54 * Results!$B$6</f>
+        <f>Source!C54</f>
         <v>5</v>
       </c>
       <c r="C11">
@@ -7104,7 +7251,7 @@
         <v>DoubleRailGun</v>
       </c>
       <c r="B12">
-        <f>Source!C55 * Results!$B$6</f>
+        <f>Source!C55</f>
         <v>5</v>
       </c>
       <c r="C12">
@@ -7134,7 +7281,7 @@
         <v>TripleRailGun</v>
       </c>
       <c r="B13">
-        <f>Source!C56 * Results!$B$6</f>
+        <f>Source!C56</f>
         <v>8</v>
       </c>
       <c r="C13">
@@ -7164,7 +7311,7 @@
         <v>SkirmishGun1</v>
       </c>
       <c r="B14">
-        <f>Source!C57 * Results!$B$6</f>
+        <f>Source!C57</f>
         <v>6</v>
       </c>
       <c r="C14">
@@ -7194,7 +7341,7 @@
         <v>SniperRifle</v>
       </c>
       <c r="B15">
-        <f>Source!C58 * Results!$B$6</f>
+        <f>Source!C58</f>
         <v>8</v>
       </c>
       <c r="C15">
@@ -7224,7 +7371,7 @@
         <v>PlasmaCannon</v>
       </c>
       <c r="B16">
-        <f>Source!C59 * Results!$B$6</f>
+        <f>Source!C59</f>
         <v>5</v>
       </c>
       <c r="C16">
@@ -7254,7 +7401,7 @@
         <v>PlasmaRifle</v>
       </c>
       <c r="B17">
-        <f>Source!C60 * Results!$B$6</f>
+        <f>Source!C60</f>
         <v>4</v>
       </c>
       <c r="C17">
@@ -7284,7 +7431,7 @@
         <v>TachyonCannon</v>
       </c>
       <c r="B18">
-        <f>Source!C61 * Results!$B$6</f>
+        <f>Source!C61</f>
         <v>8</v>
       </c>
       <c r="C18">
@@ -7314,7 +7461,7 @@
         <v>FortressCannon</v>
       </c>
       <c r="B19">
-        <f>Source!C62 * Results!$B$6</f>
+        <f>Source!C62</f>
         <v>7</v>
       </c>
       <c r="C19">
@@ -7344,7 +7491,7 @@
         <v>CycloneCannon</v>
       </c>
       <c r="B20">
-        <f>Source!C63 * Results!$B$6</f>
+        <f>Source!C63</f>
         <v>6</v>
       </c>
       <c r="C20">
@@ -7374,7 +7521,7 @@
         <v>SuicideNuke</v>
       </c>
       <c r="B21">
-        <f>Source!C64 * Results!$B$6</f>
+        <f>Source!C64</f>
         <v>2</v>
       </c>
       <c r="C21">
@@ -7404,7 +7551,7 @@
         <v>PhaseTankCannon</v>
       </c>
       <c r="B22">
-        <f>Source!C65 * Results!$B$6</f>
+        <f>Source!C65</f>
         <v>6</v>
       </c>
       <c r="C22">
@@ -7434,7 +7581,7 @@
         <v>LaserCannon</v>
       </c>
       <c r="B23">
-        <f>Source!C66 * Results!$B$6</f>
+        <f>Source!C66</f>
         <v>6</v>
       </c>
       <c r="C23">
@@ -7464,7 +7611,7 @@
         <v>FixedGroundToAirLaser</v>
       </c>
       <c r="B24">
-        <f>Source!C67 * Results!$B$6</f>
+        <f>Source!C67</f>
         <v>20</v>
       </c>
       <c r="C24">
@@ -7494,7 +7641,7 @@
         <v>IMPFixedGroundToAirLaser</v>
       </c>
       <c r="B25">
-        <f>Source!C68 * Results!$B$6</f>
+        <f>Source!C68</f>
         <v>10</v>
       </c>
       <c r="C25">
@@ -7524,7 +7671,7 @@
         <v>FixedLaserPlat</v>
       </c>
       <c r="B26">
-        <f>Source!C69 * Results!$B$6</f>
+        <f>Source!C69</f>
         <v>9</v>
       </c>
       <c r="C26">
@@ -7554,7 +7701,7 @@
         <v>GroundToAirLaser</v>
       </c>
       <c r="B27">
-        <f>Source!C70 * Results!$B$6</f>
+        <f>Source!C70</f>
         <v>8</v>
       </c>
       <c r="C27">
@@ -7584,7 +7731,7 @@
         <v>BkLaser</v>
       </c>
       <c r="B28">
-        <f>Source!C71 * Results!$B$6</f>
+        <f>Source!C71</f>
         <v>5</v>
       </c>
       <c r="C28">
@@ -7614,7 +7761,7 @@
         <v>GatLaser</v>
       </c>
       <c r="B29">
-        <f>Source!C72 * Results!$B$6</f>
+        <f>Source!C72</f>
         <v>5</v>
       </c>
       <c r="C29">
@@ -7644,7 +7791,7 @@
         <v>GatPlasma</v>
       </c>
       <c r="B30">
-        <f>Source!C73 * Results!$B$6</f>
+        <f>Source!C73</f>
         <v>5</v>
       </c>
       <c r="C30">
@@ -7674,7 +7821,7 @@
         <v>PolyAcid</v>
       </c>
       <c r="B31">
-        <f>Source!C74 * Results!$B$6</f>
+        <f>Source!C74</f>
         <v>5</v>
       </c>
       <c r="C31">
@@ -7704,7 +7851,7 @@
         <v>TankHunterGun</v>
       </c>
       <c r="B32">
-        <f>Source!C75 * Results!$B$6</f>
+        <f>Source!C75</f>
         <v>3</v>
       </c>
       <c r="C32">
@@ -7734,7 +7881,7 @@
         <v>OutriderMissile</v>
       </c>
       <c r="B33">
-        <f>Source!C76 * Results!$B$6</f>
+        <f>Source!C76</f>
         <v>5</v>
       </c>
       <c r="C33">
@@ -7764,7 +7911,7 @@
         <v>ArtilleryShell</v>
       </c>
       <c r="B34">
-        <f>Source!C77 * Results!$B$6</f>
+        <f>Source!C77</f>
         <v>45</v>
       </c>
       <c r="C34">
@@ -7794,7 +7941,7 @@
         <v>IMPArtilleryShell</v>
       </c>
       <c r="B35">
-        <f>Source!C78 * Results!$B$6</f>
+        <f>Source!C78</f>
         <v>45</v>
       </c>
       <c r="C35">
@@ -7824,7 +7971,7 @@
         <v>MedicHeal</v>
       </c>
       <c r="B36">
-        <f>Source!C79 * Results!$B$6</f>
+        <f>Source!C79</f>
         <v>1</v>
       </c>
       <c r="C36">
@@ -7854,7 +8001,7 @@
         <v>AmperAmp</v>
       </c>
       <c r="B37">
-        <f>Source!C80 * Results!$B$6</f>
+        <f>Source!C80</f>
         <v>5</v>
       </c>
       <c r="C37">
@@ -7884,7 +8031,7 @@
         <v>MechanicRepair</v>
       </c>
       <c r="B38">
-        <f>Source!C81 * Results!$B$6</f>
+        <f>Source!C81</f>
         <v>1</v>
       </c>
       <c r="C38">
@@ -7914,7 +8061,7 @@
         <v>SelfDestruct1</v>
       </c>
       <c r="B39">
-        <f>Source!C82 * Results!$B$6</f>
+        <f>Source!C82</f>
         <v>1</v>
       </c>
       <c r="C39">
@@ -7944,7 +8091,7 @@
         <v>NoWeapon</v>
       </c>
       <c r="B40">
-        <f>Source!C83 * Results!$B$6</f>
+        <f>Source!C83</f>
         <v>10</v>
       </c>
       <c r="C40">
@@ -7974,7 +8121,7 @@
         <v>TemporalRift</v>
       </c>
       <c r="B41">
-        <f>Source!C84 * Results!$B$6</f>
+        <f>Source!C84</f>
         <v>350</v>
       </c>
       <c r="C41">
@@ -8004,7 +8151,7 @@
         <v>SeismicWave</v>
       </c>
       <c r="B42">
-        <f>Source!C85 * Results!$B$6</f>
+        <f>Source!C85</f>
         <v>24</v>
       </c>
       <c r="C42">
@@ -8034,7 +8181,7 @@
         <v>NeutronAss</v>
       </c>
       <c r="B43">
-        <f>Source!C86 * Results!$B$6</f>
+        <f>Source!C86</f>
         <v>9</v>
       </c>
       <c r="C43">
@@ -8064,7 +8211,7 @@
         <v>Shredder</v>
       </c>
       <c r="B44">
-        <f>Source!C87 * Results!$B$6</f>
+        <f>Source!C87</f>
         <v>1</v>
       </c>
       <c r="C44">
@@ -8094,7 +8241,7 @@
         <v>Contaminator</v>
       </c>
       <c r="B45">
-        <f>Source!C88 * Results!$B$6</f>
+        <f>Source!C88</f>
         <v>1</v>
       </c>
       <c r="C45">
@@ -8124,7 +8271,7 @@
         <v>LaserPistol</v>
       </c>
       <c r="B46">
-        <f>Source!C89 * Results!$B$6</f>
+        <f>Source!C89</f>
         <v>3</v>
       </c>
       <c r="C46">
@@ -8148,7 +8295,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>0</v>
       </c>
@@ -8159,10 +8306,13 @@
         <v>9</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+        <v>317</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
         <f>Source!A96</f>
         <v>FGConstructionCrew</v>
@@ -8179,8 +8329,12 @@
         <f>Source!G96*Results!$B$5</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61">
+        <f>Source!I96 * Results!$B$6</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
         <f>Source!A97</f>
         <v>FGGroundTransporter</v>
@@ -8197,8 +8351,12 @@
         <f>Source!G97*Results!$B$5</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62">
+        <f>Source!I97 * Results!$B$6</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
         <f>Source!A98</f>
         <v>FGHoverTransporter</v>
@@ -8215,8 +8373,12 @@
         <f>Source!G98*Results!$B$5</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63">
+        <f>Source!I98 * Results!$B$6</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
         <f>Source!A99</f>
         <v>FGFreedomFighter</v>
@@ -8233,8 +8395,12 @@
         <f>Source!G99*Results!$B$5</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64">
+        <f>Source!I99 * Results!$B$6</f>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f>Source!A100</f>
         <v>FGMercenary</v>
@@ -8251,8 +8417,12 @@
         <f>Source!G100*Results!$B$5</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65">
+        <f>Source!I100 * Results!$B$6</f>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f>Source!A101</f>
         <v>FGSniper</v>
@@ -8269,8 +8439,12 @@
         <f>Source!G101*Results!$B$5</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66">
+        <f>Source!I101 * Results!$B$6</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f>Source!A102</f>
         <v>FGScout</v>
@@ -8287,8 +8461,12 @@
         <f>Source!G102*Results!$B$5</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67">
+        <f>Source!I102 * Results!$B$6</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f>Source!A103</f>
         <v>FGMedic</v>
@@ -8305,8 +8483,12 @@
         <f>Source!G103*Results!$B$5</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68">
+        <f>Source!I103 * Results!$B$6</f>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
         <f>Source!A104</f>
         <v>FGSaboteur</v>
@@ -8323,8 +8505,12 @@
         <f>Source!G104*Results!$B$5</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69">
+        <f>Source!I104 * Results!$B$6</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
         <f>Source!A105</f>
         <v>FGMechanic</v>
@@ -8341,8 +8527,12 @@
         <f>Source!G105*Results!$B$5</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70">
+        <f>Source!I105 * Results!$B$6</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
         <f>Source!A106</f>
         <v>FGSuicideNuker</v>
@@ -8359,8 +8549,12 @@
         <f>Source!G106*Results!$B$5</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71">
+        <f>Source!I106 * Results!$B$6</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
         <f>Source!A107</f>
         <v>FGSpy</v>
@@ -8377,8 +8571,12 @@
         <f>Source!G107*Results!$B$5</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72">
+        <f>Source!I107 * Results!$B$6</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
         <f>Source!A108</f>
         <v>FGSpiderBike</v>
@@ -8395,8 +8593,12 @@
         <f>Source!G108*Results!$B$5</f>
         <v>80</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73">
+        <f>Source!I108 * Results!$B$6</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
         <f>Source!A109</f>
         <v>FGIFV</v>
@@ -8413,8 +8615,12 @@
         <f>Source!G109*Results!$B$5</f>
         <v>144</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74">
+        <f>Source!I109 * Results!$B$6</f>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
         <f>Source!A110</f>
         <v>FGMediumTank</v>
@@ -8431,8 +8637,12 @@
         <f>Source!G110*Results!$B$5</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75">
+        <f>Source!I110 * Results!$B$6</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
         <f>Source!A111</f>
         <v>FGTankHunterTank</v>
@@ -8449,8 +8659,12 @@
         <f>Source!G111*Results!$B$5</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76">
+        <f>Source!I111 * Results!$B$6</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
         <f>Source!A112</f>
         <v>FGAmbushTank</v>
@@ -8467,8 +8681,12 @@
         <f>Source!G112*Results!$B$5</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77">
+        <f>Source!I112 * Results!$B$6</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="str">
         <f>Source!A113</f>
         <v>FGConstructionMAD</v>
@@ -8485,8 +8703,12 @@
         <f>Source!G113*Results!$B$5</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78">
+        <f>Source!I113 * Results!$B$6</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
         <f>Source!A114</f>
         <v>FGTripleRailHoverTank</v>
@@ -8503,8 +8725,12 @@
         <f>Source!G114*Results!$B$5</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79">
+        <f>Source!I114 * Results!$B$6</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="str">
         <f>Source!A115</f>
         <v>FGSPA</v>
@@ -8521,8 +8747,12 @@
         <f>Source!G115*Results!$B$5</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80">
+        <f>Source!I115 * Results!$B$6</f>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="str">
         <f>Source!A116</f>
         <v>FGSkyBike</v>
@@ -8539,8 +8769,12 @@
         <f>Source!G116*Results!$B$5</f>
         <v>128</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81">
+        <f>Source!I116 * Results!$B$6</f>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="str">
         <f>Source!A117</f>
         <v>FGDualSkyBike</v>
@@ -8557,8 +8791,12 @@
         <f>Source!G117*Results!$B$5</f>
         <v>128</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82">
+        <f>Source!I117 * Results!$B$6</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="str">
         <f>Source!A118</f>
         <v>FGShockWave</v>
@@ -8575,8 +8813,12 @@
         <f>Source!G118*Results!$B$5</f>
         <v>80</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83">
+        <f>Source!I118 * Results!$B$6</f>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="str">
         <f>Source!A119</f>
         <v>FGContaminator</v>
@@ -8593,8 +8835,12 @@
         <f>Source!G119*Results!$B$5</f>
         <v>64</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84">
+        <f>Source!I119 * Results!$B$6</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="str">
         <f>Source!A120</f>
         <v>FGundergtunnel</v>
@@ -8611,8 +8857,12 @@
         <f>Source!G120*Results!$B$5</f>
         <v>144</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85">
+        <f>Source!I120 * Results!$B$6</f>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="str">
         <f>Source!A121</f>
         <v>FGAntiAirSite</v>
@@ -8629,8 +8879,12 @@
         <f>Source!G121*Results!$B$5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E86">
+        <f>Source!I121 * Results!$B$6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="str">
         <f>Source!A122</f>
         <v>FGGuardTower</v>
@@ -8647,8 +8901,12 @@
         <f>Source!G122*Results!$B$5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87">
+        <f>Source!I122 * Results!$B$6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="str">
         <f>Source!A123</f>
         <v>FGAdvancedGuardTower</v>
@@ -8665,8 +8923,12 @@
         <f>Source!G123*Results!$B$5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E88">
+        <f>Source!I123 * Results!$B$6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="str">
         <f>Source!A124</f>
         <v>FGBaseMover</v>
@@ -8683,8 +8945,12 @@
         <f>Source!G124*Results!$B$5</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E89">
+        <f>Source!I124 * Results!$B$6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="str">
         <f>Source!A125</f>
         <v>IMPConstructionCrew</v>
@@ -8701,8 +8967,12 @@
         <f>Source!G125*Results!$B$5</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90">
+        <f>Source!I125 * Results!$B$6</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="str">
         <f>Source!A126</f>
         <v>ImpGroundTransporter</v>
@@ -8719,8 +8989,12 @@
         <f>Source!G126*Results!$B$5</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E91">
+        <f>Source!I126 * Results!$B$6</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="str">
         <f>Source!A127</f>
         <v>ImpHoverTransporter</v>
@@ -8737,8 +9011,12 @@
         <f>Source!G127*Results!$B$5</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92">
+        <f>Source!I127 * Results!$B$6</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="str">
         <f>Source!A128</f>
         <v>IMPStrikeMarine</v>
@@ -8755,8 +9033,12 @@
         <f>Source!G128*Results!$B$5</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93">
+        <f>Source!I128 * Results!$B$6</f>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="str">
         <f>Source!A129</f>
         <v>IMPFireSupportMarine</v>
@@ -8773,8 +9055,12 @@
         <f>Source!G129*Results!$B$5</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E94">
+        <f>Source!I129 * Results!$B$6</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="str">
         <f>Source!A130</f>
         <v>IMPHoverMarine</v>
@@ -8791,8 +9077,12 @@
         <f>Source!G130*Results!$B$5</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E95">
+        <f>Source!I130 * Results!$B$6</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="str">
         <f>Source!A131</f>
         <v>IMPSpy</v>
@@ -8809,8 +9099,12 @@
         <f>Source!G131*Results!$B$5</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96">
+        <f>Source!I131 * Results!$B$6</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="str">
         <f>Source!A132</f>
         <v>IMPSuicideZombie</v>
@@ -8827,8 +9121,12 @@
         <f>Source!G132*Results!$B$5</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97">
+        <f>Source!I132 * Results!$B$6</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="str">
         <f>Source!A133</f>
         <v>IMPScoutTank</v>
@@ -8845,8 +9143,12 @@
         <f>Source!G133*Results!$B$5</f>
         <v>88</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E98">
+        <f>Source!I133 * Results!$B$6</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="str">
         <f>Source!A134</f>
         <v>IMPAssaultVehicle</v>
@@ -8863,8 +9165,12 @@
         <f>Source!G134*Results!$B$5</f>
         <v>80</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99">
+        <f>Source!I134 * Results!$B$6</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="str">
         <f>Source!A135</f>
         <v>IMPPlasmaTank</v>
@@ -8881,8 +9187,12 @@
         <f>Source!G135*Results!$B$5</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E100">
+        <f>Source!I135 * Results!$B$6</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="str">
         <f>Source!A136</f>
         <v>IMPAmper</v>
@@ -8899,8 +9209,12 @@
         <f>Source!G136*Results!$B$5</f>
         <v>64</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E101">
+        <f>Source!I136 * Results!$B$6</f>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="str">
         <f>Source!A137</f>
         <v>IMPMAD</v>
@@ -8917,8 +9231,12 @@
         <f>Source!G137*Results!$B$5</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E102">
+        <f>Source!I137 * Results!$B$6</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="str">
         <f>Source!A138</f>
         <v>IMPReconSaucer</v>
@@ -8935,8 +9253,12 @@
         <f>Source!G138*Results!$B$5</f>
         <v>96</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E103">
+        <f>Source!I138 * Results!$B$6</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="str">
         <f>Source!A139</f>
         <v>IMPShredder</v>
@@ -8953,8 +9275,12 @@
         <f>Source!G139*Results!$B$5</f>
         <v>80</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E104">
+        <f>Source!I139 * Results!$B$6</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="str">
         <f>Source!A140</f>
         <v>IMPHostageTaker</v>
@@ -8971,8 +9297,12 @@
         <f>Source!G140*Results!$B$5</f>
         <v>80</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E105">
+        <f>Source!I140 * Results!$B$6</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="str">
         <f>Source!A141</f>
         <v>IMPTachyonTank</v>
@@ -8989,8 +9319,12 @@
         <f>Source!G141*Results!$B$5</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E106">
+        <f>Source!I141 * Results!$B$6</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="str">
         <f>Source!A142</f>
         <v>IMPShieldedSPA</v>
@@ -9007,8 +9341,12 @@
         <f>Source!G142*Results!$B$5</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E107">
+        <f>Source!I142 * Results!$B$6</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="str">
         <f>Source!A143</f>
         <v>IMPSPA</v>
@@ -9025,8 +9363,12 @@
         <f>Source!G143*Results!$B$5</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E108">
+        <f>Source!I143 * Results!$B$6</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="str">
         <f>Source!A144</f>
         <v>ImpVTOL</v>
@@ -9043,8 +9385,12 @@
         <f>Source!G144*Results!$B$5</f>
         <v>128</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E109">
+        <f>Source!I144 * Results!$B$6</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="str">
         <f>Source!A145</f>
         <v>IMPSkyFortress</v>
@@ -9061,8 +9407,12 @@
         <f>Source!G145*Results!$B$5</f>
         <v>80</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E110">
+        <f>Source!I145 * Results!$B$6</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="str">
         <f>Source!A146</f>
         <v>IMPContaminator</v>
@@ -9079,8 +9429,12 @@
         <f>Source!G146*Results!$B$5</f>
         <v>64</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E111">
+        <f>Source!I146 * Results!$B$6</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="str">
         <f>Source!A147</f>
         <v>IMPAntiAirSite</v>
@@ -9097,8 +9451,12 @@
         <f>Source!G147*Results!$B$5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E112">
+        <f>Source!I147 * Results!$B$6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="str">
         <f>Source!A148</f>
         <v>IMPGuardTower</v>
@@ -9115,8 +9473,12 @@
         <f>Source!G148*Results!$B$5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E113">
+        <f>Source!I148 * Results!$B$6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="str">
         <f>Source!A149</f>
         <v>IMPAdvancedGuardTower</v>
@@ -9133,8 +9495,12 @@
         <f>Source!G149*Results!$B$5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E114">
+        <f>Source!I149 * Results!$B$6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="str">
         <f>Source!A150</f>
         <v>IMPriftCreator</v>
@@ -9151,8 +9517,12 @@
         <f>Source!G150*Results!$B$5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E115">
+        <f>Source!I150 * Results!$B$6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="str">
         <f>Source!A151</f>
         <v>CameraTower</v>
@@ -9167,6 +9537,10 @@
       </c>
       <c r="D116">
         <f>Source!G151*Results!$B$5</f>
+        <v>0</v>
+      </c>
+      <c r="E116">
+        <f>Source!I151 * Results!$B$6</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Altered all weapons to have a 1.4 factor delay. Made infantry crushable by shredder. Made exterminator non-crushable.
</commit_message>
<xml_diff>
--- a/mods/dr/The Spreadsheet.xlsx
+++ b/mods/dr/The Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8D9CB213-48F0-430C-A113-BA46C527A65C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{ABA966CE-318F-4CC3-A5F3-5472C395CA0A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="3225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2044,8 +2044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B115" workbookViewId="0">
-      <selection activeCell="I146" sqref="I146"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7077,8 +7077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD92D53-EC10-4CE0-957A-62D9B9206E5C}">
   <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7113,7 +7113,7 @@
         <v>525</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -7129,7 +7129,7 @@
         <v>528</v>
       </c>
       <c r="B6">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7165,8 +7165,8 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <f>Source!D52*Results!$B$4</f>
-        <v>15</v>
+        <f>ROUND(Source!D52*Results!$B$4, 0)</f>
+        <v>21</v>
       </c>
       <c r="D9" s="8">
         <f>Source!E52*Results!$B$3</f>
@@ -7195,8 +7195,8 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <f>Source!D53*Results!$B$4</f>
-        <v>8</v>
+        <f>ROUND(Source!D53*Results!$B$4, 0)</f>
+        <v>11</v>
       </c>
       <c r="D10" s="8">
         <f>Source!E53*Results!$B$3</f>
@@ -7225,8 +7225,8 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <f>Source!D54*Results!$B$4</f>
-        <v>11</v>
+        <f>ROUND(Source!D54*Results!$B$4, 0)</f>
+        <v>15</v>
       </c>
       <c r="D11" s="8">
         <f>Source!E54*Results!$B$3</f>
@@ -7255,8 +7255,8 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <f>Source!D55*Results!$B$4</f>
-        <v>13</v>
+        <f>ROUND(Source!D55*Results!$B$4, 0)</f>
+        <v>18</v>
       </c>
       <c r="D12" s="8">
         <f>Source!E55*Results!$B$3</f>
@@ -7285,8 +7285,8 @@
         <v>8</v>
       </c>
       <c r="C13">
-        <f>Source!D56*Results!$B$4</f>
-        <v>20</v>
+        <f>ROUND(Source!D56*Results!$B$4, 0)</f>
+        <v>28</v>
       </c>
       <c r="D13" s="8">
         <f>Source!E56*Results!$B$3</f>
@@ -7315,8 +7315,8 @@
         <v>6</v>
       </c>
       <c r="C14">
-        <f>Source!D57*Results!$B$4</f>
-        <v>20</v>
+        <f>ROUND(Source!D57*Results!$B$4, 0)</f>
+        <v>28</v>
       </c>
       <c r="D14" s="8">
         <f>Source!E57*Results!$B$3</f>
@@ -7345,8 +7345,8 @@
         <v>8</v>
       </c>
       <c r="C15">
-        <f>Source!D58*Results!$B$4</f>
-        <v>50</v>
+        <f>ROUND(Source!D58*Results!$B$4, 0)</f>
+        <v>70</v>
       </c>
       <c r="D15" s="8">
         <f>Source!E58*Results!$B$3</f>
@@ -7375,8 +7375,8 @@
         <v>5</v>
       </c>
       <c r="C16">
-        <f>Source!D59*Results!$B$4</f>
-        <v>15</v>
+        <f>ROUND(Source!D59*Results!$B$4, 0)</f>
+        <v>21</v>
       </c>
       <c r="D16" s="8">
         <f>Source!E59*Results!$B$3</f>
@@ -7405,8 +7405,8 @@
         <v>4</v>
       </c>
       <c r="C17">
-        <f>Source!D60*Results!$B$4</f>
-        <v>8</v>
+        <f>ROUND(Source!D60*Results!$B$4, 0)</f>
+        <v>11</v>
       </c>
       <c r="D17" s="8">
         <f>Source!E60*Results!$B$3</f>
@@ -7435,8 +7435,8 @@
         <v>8</v>
       </c>
       <c r="C18">
-        <f>Source!D61*Results!$B$4</f>
-        <v>20</v>
+        <f>ROUND(Source!D61*Results!$B$4, 0)</f>
+        <v>28</v>
       </c>
       <c r="D18" s="8">
         <f>Source!E61*Results!$B$3</f>
@@ -7465,8 +7465,8 @@
         <v>7</v>
       </c>
       <c r="C19">
-        <f>Source!D62*Results!$B$4</f>
-        <v>20</v>
+        <f>ROUND(Source!D62*Results!$B$4, 0)</f>
+        <v>28</v>
       </c>
       <c r="D19" s="8">
         <f>Source!E62*Results!$B$3</f>
@@ -7495,8 +7495,8 @@
         <v>6</v>
       </c>
       <c r="C20">
-        <f>Source!D63*Results!$B$4</f>
-        <v>10</v>
+        <f>ROUND(Source!D63*Results!$B$4, 0)</f>
+        <v>14</v>
       </c>
       <c r="D20" s="8">
         <f>Source!E63*Results!$B$3</f>
@@ -7525,8 +7525,8 @@
         <v>2</v>
       </c>
       <c r="C21">
-        <f>Source!D64*Results!$B$4</f>
-        <v>50</v>
+        <f>ROUND(Source!D64*Results!$B$4, 0)</f>
+        <v>70</v>
       </c>
       <c r="D21" s="8">
         <f>Source!E64*Results!$B$3</f>
@@ -7555,8 +7555,8 @@
         <v>6</v>
       </c>
       <c r="C22">
-        <f>Source!D65*Results!$B$4</f>
-        <v>13</v>
+        <f>ROUND(Source!D65*Results!$B$4, 0)</f>
+        <v>18</v>
       </c>
       <c r="D22" s="8">
         <f>Source!E65*Results!$B$3</f>
@@ -7585,8 +7585,8 @@
         <v>6</v>
       </c>
       <c r="C23">
-        <f>Source!D66*Results!$B$4</f>
-        <v>13</v>
+        <f>ROUND(Source!D66*Results!$B$4, 0)</f>
+        <v>18</v>
       </c>
       <c r="D23" s="8">
         <f>Source!E66*Results!$B$3</f>
@@ -7615,8 +7615,8 @@
         <v>20</v>
       </c>
       <c r="C24">
-        <f>Source!D67*Results!$B$4</f>
-        <v>14</v>
+        <f>ROUND(Source!D67*Results!$B$4, 0)</f>
+        <v>20</v>
       </c>
       <c r="D24" s="8">
         <f>Source!E67*Results!$B$3</f>
@@ -7645,8 +7645,8 @@
         <v>10</v>
       </c>
       <c r="C25">
-        <f>Source!D68*Results!$B$4</f>
-        <v>14</v>
+        <f>ROUND(Source!D68*Results!$B$4, 0)</f>
+        <v>20</v>
       </c>
       <c r="D25" s="8">
         <f>Source!E68*Results!$B$3</f>
@@ -7675,8 +7675,8 @@
         <v>9</v>
       </c>
       <c r="C26">
-        <f>Source!D69*Results!$B$4</f>
-        <v>10</v>
+        <f>ROUND(Source!D69*Results!$B$4, 0)</f>
+        <v>14</v>
       </c>
       <c r="D26" s="8">
         <f>Source!E69*Results!$B$3</f>
@@ -7705,8 +7705,8 @@
         <v>8</v>
       </c>
       <c r="C27">
-        <f>Source!D70*Results!$B$4</f>
-        <v>20</v>
+        <f>ROUND(Source!D70*Results!$B$4, 0)</f>
+        <v>28</v>
       </c>
       <c r="D27" s="8">
         <f>Source!E70*Results!$B$3</f>
@@ -7735,8 +7735,8 @@
         <v>5</v>
       </c>
       <c r="C28">
-        <f>Source!D71*Results!$B$4</f>
-        <v>7</v>
+        <f>ROUND(Source!D71*Results!$B$4, 0)</f>
+        <v>10</v>
       </c>
       <c r="D28" s="8">
         <f>Source!E71*Results!$B$3</f>
@@ -7765,8 +7765,8 @@
         <v>5</v>
       </c>
       <c r="C29">
-        <f>Source!D72*Results!$B$4</f>
-        <v>3</v>
+        <f>ROUND(Source!D72*Results!$B$4, 0)</f>
+        <v>4</v>
       </c>
       <c r="D29" s="8">
         <f>Source!E72*Results!$B$3</f>
@@ -7795,8 +7795,8 @@
         <v>5</v>
       </c>
       <c r="C30">
-        <f>Source!D73*Results!$B$4</f>
-        <v>3</v>
+        <f>ROUND(Source!D73*Results!$B$4, 0)</f>
+        <v>4</v>
       </c>
       <c r="D30" s="8">
         <f>Source!E73*Results!$B$3</f>
@@ -7825,8 +7825,8 @@
         <v>5</v>
       </c>
       <c r="C31">
-        <f>Source!D74*Results!$B$4</f>
-        <v>20</v>
+        <f>ROUND(Source!D74*Results!$B$4, 0)</f>
+        <v>28</v>
       </c>
       <c r="D31" s="8">
         <f>Source!E74*Results!$B$3</f>
@@ -7855,8 +7855,8 @@
         <v>3</v>
       </c>
       <c r="C32">
-        <f>Source!D75*Results!$B$4</f>
-        <v>20</v>
+        <f>ROUND(Source!D75*Results!$B$4, 0)</f>
+        <v>28</v>
       </c>
       <c r="D32" s="8">
         <f>Source!E75*Results!$B$3</f>
@@ -7885,8 +7885,8 @@
         <v>5</v>
       </c>
       <c r="C33">
-        <f>Source!D76*Results!$B$4</f>
-        <v>10</v>
+        <f>ROUND(Source!D76*Results!$B$4, 0)</f>
+        <v>14</v>
       </c>
       <c r="D33" s="8">
         <f>Source!E76*Results!$B$3</f>
@@ -7915,8 +7915,8 @@
         <v>45</v>
       </c>
       <c r="C34">
-        <f>Source!D77*Results!$B$4</f>
-        <v>80</v>
+        <f>ROUND(Source!D77*Results!$B$4, 0)</f>
+        <v>112</v>
       </c>
       <c r="D34" s="8">
         <f>Source!E77*Results!$B$3</f>
@@ -7945,8 +7945,8 @@
         <v>45</v>
       </c>
       <c r="C35">
-        <f>Source!D78*Results!$B$4</f>
-        <v>80</v>
+        <f>ROUND(Source!D78*Results!$B$4, 0)</f>
+        <v>112</v>
       </c>
       <c r="D35" s="8">
         <f>Source!E78*Results!$B$3</f>
@@ -7975,8 +7975,8 @@
         <v>1</v>
       </c>
       <c r="C36">
-        <f>Source!D79*Results!$B$4</f>
-        <v>10</v>
+        <f>ROUND(Source!D79*Results!$B$4, 0)</f>
+        <v>14</v>
       </c>
       <c r="D36" s="8">
         <f>Source!E79*Results!$B$3</f>
@@ -8005,8 +8005,8 @@
         <v>5</v>
       </c>
       <c r="C37">
-        <f>Source!D80*Results!$B$4</f>
-        <v>10</v>
+        <f>ROUND(Source!D80*Results!$B$4, 0)</f>
+        <v>14</v>
       </c>
       <c r="D37" s="8">
         <f>Source!E80*Results!$B$3</f>
@@ -8035,8 +8035,8 @@
         <v>1</v>
       </c>
       <c r="C38">
-        <f>Source!D81*Results!$B$4</f>
-        <v>10</v>
+        <f>ROUND(Source!D81*Results!$B$4, 0)</f>
+        <v>14</v>
       </c>
       <c r="D38" s="8">
         <f>Source!E81*Results!$B$3</f>
@@ -8065,7 +8065,7 @@
         <v>1</v>
       </c>
       <c r="C39">
-        <f>Source!D82*Results!$B$4</f>
+        <f>ROUND(Source!D82*Results!$B$4, 0)</f>
         <v>1</v>
       </c>
       <c r="D39" s="8">
@@ -8095,8 +8095,8 @@
         <v>10</v>
       </c>
       <c r="C40">
-        <f>Source!D83*Results!$B$4</f>
-        <v>10</v>
+        <f>ROUND(Source!D83*Results!$B$4, 0)</f>
+        <v>14</v>
       </c>
       <c r="D40" s="8">
         <f>Source!E83*Results!$B$3</f>
@@ -8125,7 +8125,7 @@
         <v>350</v>
       </c>
       <c r="C41">
-        <f>Source!D84*Results!$B$4</f>
+        <f>ROUND(Source!D84*Results!$B$4, 0)</f>
         <v>1</v>
       </c>
       <c r="D41" s="8">
@@ -8155,7 +8155,7 @@
         <v>24</v>
       </c>
       <c r="C42">
-        <f>Source!D85*Results!$B$4</f>
+        <f>ROUND(Source!D85*Results!$B$4, 0)</f>
         <v>0</v>
       </c>
       <c r="D42" s="8">
@@ -8185,8 +8185,8 @@
         <v>9</v>
       </c>
       <c r="C43">
-        <f>Source!D86*Results!$B$4</f>
-        <v>32</v>
+        <f>ROUND(Source!D86*Results!$B$4, 0)</f>
+        <v>45</v>
       </c>
       <c r="D43" s="8">
         <f>Source!E86*Results!$B$3</f>
@@ -8215,7 +8215,7 @@
         <v>1</v>
       </c>
       <c r="C44">
-        <f>Source!D87*Results!$B$4</f>
+        <f>ROUND(Source!D87*Results!$B$4, 0)</f>
         <v>0</v>
       </c>
       <c r="D44" s="8">
@@ -8245,8 +8245,8 @@
         <v>1</v>
       </c>
       <c r="C45">
-        <f>Source!D88*Results!$B$4</f>
-        <v>2</v>
+        <f>ROUND(Source!D88*Results!$B$4, 0)</f>
+        <v>3</v>
       </c>
       <c r="D45" s="8">
         <f>Source!E88*Results!$B$3</f>
@@ -8275,8 +8275,8 @@
         <v>3</v>
       </c>
       <c r="C46">
-        <f>Source!D89*Results!$B$4</f>
-        <v>5</v>
+        <f>ROUND(Source!D89*Results!$B$4, 0)</f>
+        <v>7</v>
       </c>
       <c r="D46" s="8">
         <f>Source!E89*Results!$B$3</f>
@@ -8331,7 +8331,7 @@
       </c>
       <c r="E61">
         <f>Source!I96 * Results!$B$6</f>
-        <v>120</v>
+        <v>72</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -8353,7 +8353,7 @@
       </c>
       <c r="E62">
         <f>Source!I97 * Results!$B$6</f>
-        <v>200</v>
+        <v>120</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -8375,7 +8375,7 @@
       </c>
       <c r="E63">
         <f>Source!I98 * Results!$B$6</f>
-        <v>320</v>
+        <v>192</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -8397,7 +8397,7 @@
       </c>
       <c r="E64">
         <f>Source!I99 * Results!$B$6</f>
-        <v>160</v>
+        <v>96</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -8419,7 +8419,7 @@
       </c>
       <c r="E65">
         <f>Source!I100 * Results!$B$6</f>
-        <v>160</v>
+        <v>96</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -8441,7 +8441,7 @@
       </c>
       <c r="E66">
         <f>Source!I101 * Results!$B$6</f>
-        <v>240</v>
+        <v>144</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -8463,7 +8463,7 @@
       </c>
       <c r="E67">
         <f>Source!I102 * Results!$B$6</f>
-        <v>240</v>
+        <v>144</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -8485,7 +8485,7 @@
       </c>
       <c r="E68">
         <f>Source!I103 * Results!$B$6</f>
-        <v>160</v>
+        <v>96</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -8507,7 +8507,7 @@
       </c>
       <c r="E69">
         <f>Source!I104 * Results!$B$6</f>
-        <v>240</v>
+        <v>144</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -8529,7 +8529,7 @@
       </c>
       <c r="E70">
         <f>Source!I105 * Results!$B$6</f>
-        <v>240</v>
+        <v>144</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -8551,7 +8551,7 @@
       </c>
       <c r="E71">
         <f>Source!I106 * Results!$B$6</f>
-        <v>320</v>
+        <v>192</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -8573,7 +8573,7 @@
       </c>
       <c r="E72">
         <f>Source!I107 * Results!$B$6</f>
-        <v>240</v>
+        <v>144</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -8595,7 +8595,7 @@
       </c>
       <c r="E73">
         <f>Source!I108 * Results!$B$6</f>
-        <v>480</v>
+        <v>288</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -8617,7 +8617,7 @@
       </c>
       <c r="E74">
         <f>Source!I109 * Results!$B$6</f>
-        <v>360</v>
+        <v>216</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -8639,7 +8639,7 @@
       </c>
       <c r="E75">
         <f>Source!I110 * Results!$B$6</f>
-        <v>320</v>
+        <v>192</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -8661,7 +8661,7 @@
       </c>
       <c r="E76">
         <f>Source!I111 * Results!$B$6</f>
-        <v>400</v>
+        <v>240</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -8683,7 +8683,7 @@
       </c>
       <c r="E77">
         <f>Source!I112 * Results!$B$6</f>
-        <v>240</v>
+        <v>144</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -8705,7 +8705,7 @@
       </c>
       <c r="E78">
         <f>Source!I113 * Results!$B$6</f>
-        <v>240</v>
+        <v>144</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -8727,7 +8727,7 @@
       </c>
       <c r="E79">
         <f>Source!I114 * Results!$B$6</f>
-        <v>240</v>
+        <v>144</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -8749,7 +8749,7 @@
       </c>
       <c r="E80">
         <f>Source!I115 * Results!$B$6</f>
-        <v>160</v>
+        <v>96</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -8771,7 +8771,7 @@
       </c>
       <c r="E81">
         <f>Source!I116 * Results!$B$6</f>
-        <v>560</v>
+        <v>336</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -8793,7 +8793,7 @@
       </c>
       <c r="E82">
         <f>Source!I117 * Results!$B$6</f>
-        <v>480</v>
+        <v>288</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -8815,7 +8815,7 @@
       </c>
       <c r="E83">
         <f>Source!I118 * Results!$B$6</f>
-        <v>160</v>
+        <v>96</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -8837,7 +8837,7 @@
       </c>
       <c r="E84">
         <f>Source!I119 * Results!$B$6</f>
-        <v>80</v>
+        <v>48</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -8859,7 +8859,7 @@
       </c>
       <c r="E85">
         <f>Source!I120 * Results!$B$6</f>
-        <v>160</v>
+        <v>96</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -8969,7 +8969,7 @@
       </c>
       <c r="E90">
         <f>Source!I125 * Results!$B$6</f>
-        <v>120</v>
+        <v>72</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -8991,7 +8991,7 @@
       </c>
       <c r="E91">
         <f>Source!I126 * Results!$B$6</f>
-        <v>200</v>
+        <v>120</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -9013,7 +9013,7 @@
       </c>
       <c r="E92">
         <f>Source!I127 * Results!$B$6</f>
-        <v>320</v>
+        <v>192</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -9035,7 +9035,7 @@
       </c>
       <c r="E93">
         <f>Source!I128 * Results!$B$6</f>
-        <v>160</v>
+        <v>96</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -9057,7 +9057,7 @@
       </c>
       <c r="E94">
         <f>Source!I129 * Results!$B$6</f>
-        <v>120</v>
+        <v>72</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -9079,7 +9079,7 @@
       </c>
       <c r="E95">
         <f>Source!I130 * Results!$B$6</f>
-        <v>320</v>
+        <v>192</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -9101,7 +9101,7 @@
       </c>
       <c r="E96">
         <f>Source!I131 * Results!$B$6</f>
-        <v>240</v>
+        <v>144</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -9123,7 +9123,7 @@
       </c>
       <c r="E97">
         <f>Source!I132 * Results!$B$6</f>
-        <v>120</v>
+        <v>72</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -9145,7 +9145,7 @@
       </c>
       <c r="E98">
         <f>Source!I133 * Results!$B$6</f>
-        <v>400</v>
+        <v>240</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -9167,7 +9167,7 @@
       </c>
       <c r="E99">
         <f>Source!I134 * Results!$B$6</f>
-        <v>400</v>
+        <v>240</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -9189,7 +9189,7 @@
       </c>
       <c r="E100">
         <f>Source!I135 * Results!$B$6</f>
-        <v>320</v>
+        <v>192</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -9211,7 +9211,7 @@
       </c>
       <c r="E101">
         <f>Source!I136 * Results!$B$6</f>
-        <v>160</v>
+        <v>96</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -9233,7 +9233,7 @@
       </c>
       <c r="E102">
         <f>Source!I137 * Results!$B$6</f>
-        <v>320</v>
+        <v>192</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -9255,7 +9255,7 @@
       </c>
       <c r="E103">
         <f>Source!I138 * Results!$B$6</f>
-        <v>320</v>
+        <v>192</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -9277,7 +9277,7 @@
       </c>
       <c r="E104">
         <f>Source!I139 * Results!$B$6</f>
-        <v>400</v>
+        <v>240</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -9299,7 +9299,7 @@
       </c>
       <c r="E105">
         <f>Source!I140 * Results!$B$6</f>
-        <v>400</v>
+        <v>240</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -9321,7 +9321,7 @@
       </c>
       <c r="E106">
         <f>Source!I141 * Results!$B$6</f>
-        <v>240</v>
+        <v>144</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -9343,7 +9343,7 @@
       </c>
       <c r="E107">
         <f>Source!I142 * Results!$B$6</f>
-        <v>240</v>
+        <v>144</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -9365,7 +9365,7 @@
       </c>
       <c r="E108">
         <f>Source!I143 * Results!$B$6</f>
-        <v>120</v>
+        <v>72</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -9387,7 +9387,7 @@
       </c>
       <c r="E109">
         <f>Source!I144 * Results!$B$6</f>
-        <v>480</v>
+        <v>288</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -9409,7 +9409,7 @@
       </c>
       <c r="E110">
         <f>Source!I145 * Results!$B$6</f>
-        <v>200</v>
+        <v>120</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -9431,7 +9431,7 @@
       </c>
       <c r="E111">
         <f>Source!I146 * Results!$B$6</f>
-        <v>80</v>
+        <v>48</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated costs, hp, weapons, etc of expansion units.
</commit_message>
<xml_diff>
--- a/mods/dr/The Spreadsheet.xlsx
+++ b/mods/dr/The Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEBADEA-99CF-4FBA-A4E6-2FD5B57A196B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539032E0-0F2D-4609-882F-0FF56AE62029}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="572">
   <si>
     <t>Unit</t>
   </si>
@@ -1704,6 +1704,39 @@
   </si>
   <si>
     <t>Gemini Tank</t>
+  </si>
+  <si>
+    <t>Ranger</t>
+  </si>
+  <si>
+    <t>Grendel Rider</t>
+  </si>
+  <si>
+    <t>Power Spiker</t>
+  </si>
+  <si>
+    <t>EMP</t>
+  </si>
+  <si>
+    <t>ufganst0</t>
+  </si>
+  <si>
+    <t>ufganmn0</t>
+  </si>
+  <si>
+    <t>AnimalTrainer</t>
+  </si>
+  <si>
+    <t>Ratmk2</t>
+  </si>
+  <si>
+    <t>GeminiTank</t>
+  </si>
+  <si>
+    <t>Shadowblade</t>
+  </si>
+  <si>
+    <t>Terraformer</t>
   </si>
 </sst>
 </file>
@@ -2138,10 +2171,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V165"/>
+  <dimension ref="A1:V179"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="A174" sqref="A174:XFD174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7472,6 +7505,379 @@
         <v>10</v>
       </c>
     </row>
+    <row r="166" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>536</v>
+      </c>
+      <c r="C166" t="s">
+        <v>532</v>
+      </c>
+      <c r="D166">
+        <v>250</v>
+      </c>
+      <c r="E166">
+        <v>8</v>
+      </c>
+      <c r="F166">
+        <v>150</v>
+      </c>
+      <c r="G166">
+        <v>6</v>
+      </c>
+      <c r="H166">
+        <v>8</v>
+      </c>
+      <c r="I166">
+        <v>14</v>
+      </c>
+      <c r="J166" t="s">
+        <v>565</v>
+      </c>
+      <c r="K166" t="s">
+        <v>566</v>
+      </c>
+      <c r="L166">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="167" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>561</v>
+      </c>
+      <c r="B167" t="s">
+        <v>567</v>
+      </c>
+      <c r="C167" t="s">
+        <v>532</v>
+      </c>
+      <c r="D167">
+        <v>300</v>
+      </c>
+      <c r="E167">
+        <v>9</v>
+      </c>
+      <c r="F167">
+        <v>100</v>
+      </c>
+      <c r="G167">
+        <v>18</v>
+      </c>
+      <c r="H167">
+        <v>8</v>
+      </c>
+      <c r="I167">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="168" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>542</v>
+      </c>
+      <c r="C168" t="s">
+        <v>532</v>
+      </c>
+      <c r="D168">
+        <v>1100</v>
+      </c>
+      <c r="E168">
+        <v>33</v>
+      </c>
+      <c r="F168">
+        <v>250</v>
+      </c>
+      <c r="G168">
+        <v>6</v>
+      </c>
+      <c r="H168">
+        <v>9</v>
+      </c>
+      <c r="I168">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="169" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>562</v>
+      </c>
+      <c r="C169" t="s">
+        <v>532</v>
+      </c>
+      <c r="D169">
+        <v>1700</v>
+      </c>
+      <c r="E169">
+        <v>51</v>
+      </c>
+      <c r="F169">
+        <v>300</v>
+      </c>
+      <c r="G169">
+        <v>10</v>
+      </c>
+      <c r="H169">
+        <v>9</v>
+      </c>
+      <c r="I169">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="170" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>563</v>
+      </c>
+      <c r="C170" t="s">
+        <v>532</v>
+      </c>
+      <c r="D170">
+        <v>2800</v>
+      </c>
+      <c r="E170">
+        <v>84</v>
+      </c>
+      <c r="F170">
+        <v>100</v>
+      </c>
+      <c r="G170">
+        <v>5</v>
+      </c>
+      <c r="H170">
+        <v>8</v>
+      </c>
+      <c r="I170">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="171" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>531</v>
+      </c>
+      <c r="C171" t="s">
+        <v>534</v>
+      </c>
+      <c r="D171">
+        <v>400</v>
+      </c>
+      <c r="E171">
+        <v>13</v>
+      </c>
+      <c r="F171">
+        <v>175</v>
+      </c>
+      <c r="G171">
+        <v>5</v>
+      </c>
+      <c r="H171">
+        <v>8</v>
+      </c>
+      <c r="I171">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="172" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>544</v>
+      </c>
+      <c r="C172" t="s">
+        <v>534</v>
+      </c>
+      <c r="D172">
+        <v>1600</v>
+      </c>
+      <c r="E172">
+        <v>48</v>
+      </c>
+      <c r="F172">
+        <v>400</v>
+      </c>
+      <c r="G172">
+        <v>15</v>
+      </c>
+      <c r="H172">
+        <v>9</v>
+      </c>
+      <c r="I172">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="173" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>552</v>
+      </c>
+      <c r="C173" t="s">
+        <v>534</v>
+      </c>
+      <c r="D173">
+        <v>2200</v>
+      </c>
+      <c r="E173">
+        <v>66</v>
+      </c>
+      <c r="F173">
+        <v>150</v>
+      </c>
+      <c r="G173">
+        <v>10</v>
+      </c>
+      <c r="H173">
+        <v>9</v>
+      </c>
+      <c r="I173">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="174" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>553</v>
+      </c>
+      <c r="C174" t="s">
+        <v>532</v>
+      </c>
+      <c r="D174">
+        <v>2200</v>
+      </c>
+      <c r="E174">
+        <v>66</v>
+      </c>
+      <c r="F174">
+        <v>115</v>
+      </c>
+      <c r="G174">
+        <v>16</v>
+      </c>
+      <c r="H174">
+        <v>9</v>
+      </c>
+      <c r="I174">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="175" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>564</v>
+      </c>
+      <c r="C175" t="s">
+        <v>534</v>
+      </c>
+      <c r="D175">
+        <v>2600</v>
+      </c>
+      <c r="E175">
+        <v>78</v>
+      </c>
+      <c r="F175">
+        <v>150</v>
+      </c>
+      <c r="G175">
+        <v>5</v>
+      </c>
+      <c r="H175">
+        <v>9</v>
+      </c>
+      <c r="I175">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="176" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>568</v>
+      </c>
+      <c r="C176" t="s">
+        <v>532</v>
+      </c>
+      <c r="D176">
+        <v>450</v>
+      </c>
+      <c r="E176">
+        <v>14</v>
+      </c>
+      <c r="F176">
+        <v>200</v>
+      </c>
+      <c r="G176">
+        <v>18</v>
+      </c>
+      <c r="H176">
+        <v>9</v>
+      </c>
+      <c r="I176">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>569</v>
+      </c>
+      <c r="C177" t="s">
+        <v>534</v>
+      </c>
+      <c r="D177">
+        <v>700</v>
+      </c>
+      <c r="E177">
+        <v>21</v>
+      </c>
+      <c r="F177">
+        <v>340</v>
+      </c>
+      <c r="G177">
+        <v>15</v>
+      </c>
+      <c r="H177">
+        <v>9</v>
+      </c>
+      <c r="I177">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>570</v>
+      </c>
+      <c r="C178" t="s">
+        <v>534</v>
+      </c>
+      <c r="D178">
+        <v>700</v>
+      </c>
+      <c r="E178">
+        <v>21</v>
+      </c>
+      <c r="F178">
+        <v>115</v>
+      </c>
+      <c r="G178">
+        <v>10</v>
+      </c>
+      <c r="H178">
+        <v>9</v>
+      </c>
+      <c r="I178">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>571</v>
+      </c>
+      <c r="D179">
+        <v>400</v>
+      </c>
+      <c r="E179">
+        <v>12</v>
+      </c>
+      <c r="F179">
+        <v>100</v>
+      </c>
+      <c r="G179">
+        <v>5</v>
+      </c>
+      <c r="H179">
+        <v>9</v>
+      </c>
+      <c r="I179">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7480,10 +7886,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD92D53-EC10-4CE0-957A-62D9B9206E5C}">
-  <dimension ref="A1:G116"/>
+  <dimension ref="A1:G130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="K51" sqref="K51"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="A116" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10252,6 +10658,314 @@
         <v>0</v>
       </c>
     </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" t="str">
+        <f>Source!A166</f>
+        <v>Gant</v>
+      </c>
+      <c r="B117">
+        <f>Source!B166</f>
+        <v>0</v>
+      </c>
+      <c r="C117" t="str">
+        <f>Source!C166</f>
+        <v>Xenite</v>
+      </c>
+      <c r="D117">
+        <f>Source!G166*Results!$B$5</f>
+        <v>48</v>
+      </c>
+      <c r="E117">
+        <f>Source!I166 * Results!$B$6</f>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" t="str">
+        <f>Source!A167</f>
+        <v>Ranger</v>
+      </c>
+      <c r="B118" t="str">
+        <f>Source!B167</f>
+        <v>AnimalTrainer</v>
+      </c>
+      <c r="C118" t="str">
+        <f>Source!C167</f>
+        <v>Xenite</v>
+      </c>
+      <c r="D118">
+        <f>Source!G167*Results!$B$5</f>
+        <v>144</v>
+      </c>
+      <c r="E118">
+        <f>Source!I167 * Results!$B$6</f>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" t="str">
+        <f>Source!A168</f>
+        <v>Grendel</v>
+      </c>
+      <c r="B119">
+        <f>Source!B168</f>
+        <v>0</v>
+      </c>
+      <c r="C119" t="str">
+        <f>Source!C168</f>
+        <v>Xenite</v>
+      </c>
+      <c r="D119">
+        <f>Source!G168*Results!$B$5</f>
+        <v>48</v>
+      </c>
+      <c r="E119">
+        <f>Source!I168 * Results!$B$6</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" t="str">
+        <f>Source!A169</f>
+        <v>Grendel Rider</v>
+      </c>
+      <c r="B120">
+        <f>Source!B169</f>
+        <v>0</v>
+      </c>
+      <c r="C120" t="str">
+        <f>Source!C169</f>
+        <v>Xenite</v>
+      </c>
+      <c r="D120">
+        <f>Source!G169*Results!$B$5</f>
+        <v>80</v>
+      </c>
+      <c r="E120">
+        <f>Source!I169 * Results!$B$6</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" t="str">
+        <f>Source!A170</f>
+        <v>Power Spiker</v>
+      </c>
+      <c r="B121">
+        <f>Source!B170</f>
+        <v>0</v>
+      </c>
+      <c r="C121" t="str">
+        <f>Source!C170</f>
+        <v>Xenite</v>
+      </c>
+      <c r="D121">
+        <f>Source!G170*Results!$B$5</f>
+        <v>40</v>
+      </c>
+      <c r="E121">
+        <f>Source!I170 * Results!$B$6</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" t="str">
+        <f>Source!A171</f>
+        <v>Reaper</v>
+      </c>
+      <c r="B122">
+        <f>Source!B171</f>
+        <v>0</v>
+      </c>
+      <c r="C122" t="str">
+        <f>Source!C171</f>
+        <v>Shadowhand</v>
+      </c>
+      <c r="D122">
+        <f>Source!G171*Results!$B$5</f>
+        <v>40</v>
+      </c>
+      <c r="E122">
+        <f>Source!I171 * Results!$B$6</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" t="str">
+        <f>Source!A172</f>
+        <v>Fury</v>
+      </c>
+      <c r="B123">
+        <f>Source!B172</f>
+        <v>0</v>
+      </c>
+      <c r="C123" t="str">
+        <f>Source!C172</f>
+        <v>Shadowhand</v>
+      </c>
+      <c r="D123">
+        <f>Source!G172*Results!$B$5</f>
+        <v>120</v>
+      </c>
+      <c r="E123">
+        <f>Source!I172 * Results!$B$6</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" t="str">
+        <f>Source!A173</f>
+        <v>Hades Bomber</v>
+      </c>
+      <c r="B124">
+        <f>Source!B173</f>
+        <v>0</v>
+      </c>
+      <c r="C124" t="str">
+        <f>Source!C173</f>
+        <v>Shadowhand</v>
+      </c>
+      <c r="D124">
+        <f>Source!G173*Results!$B$5</f>
+        <v>80</v>
+      </c>
+      <c r="E124">
+        <f>Source!I173 * Results!$B$6</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" t="str">
+        <f>Source!A174</f>
+        <v>Avenger</v>
+      </c>
+      <c r="B125">
+        <f>Source!B174</f>
+        <v>0</v>
+      </c>
+      <c r="C125" t="str">
+        <f>Source!C174</f>
+        <v>Xenite</v>
+      </c>
+      <c r="D125">
+        <f>Source!G174*Results!$B$5</f>
+        <v>128</v>
+      </c>
+      <c r="E125">
+        <f>Source!I174 * Results!$B$6</f>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" t="str">
+        <f>Source!A175</f>
+        <v>EMP</v>
+      </c>
+      <c r="B126">
+        <f>Source!B175</f>
+        <v>0</v>
+      </c>
+      <c r="C126" t="str">
+        <f>Source!C175</f>
+        <v>Shadowhand</v>
+      </c>
+      <c r="D126">
+        <f>Source!G175*Results!$B$5</f>
+        <v>40</v>
+      </c>
+      <c r="E126">
+        <f>Source!I175 * Results!$B$6</f>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" t="str">
+        <f>Source!A176</f>
+        <v>Ratmk2</v>
+      </c>
+      <c r="B127">
+        <f>Source!B176</f>
+        <v>0</v>
+      </c>
+      <c r="C127" t="str">
+        <f>Source!C176</f>
+        <v>Xenite</v>
+      </c>
+      <c r="D127">
+        <f>Source!G176*Results!$B$5</f>
+        <v>144</v>
+      </c>
+      <c r="E127">
+        <f>Source!I176 * Results!$B$6</f>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" t="str">
+        <f>Source!A177</f>
+        <v>GeminiTank</v>
+      </c>
+      <c r="B128">
+        <f>Source!B177</f>
+        <v>0</v>
+      </c>
+      <c r="C128" t="str">
+        <f>Source!C177</f>
+        <v>Shadowhand</v>
+      </c>
+      <c r="D128">
+        <f>Source!G177*Results!$B$5</f>
+        <v>120</v>
+      </c>
+      <c r="E128">
+        <f>Source!I177 * Results!$B$6</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" t="str">
+        <f>Source!A178</f>
+        <v>Shadowblade</v>
+      </c>
+      <c r="B129">
+        <f>Source!B178</f>
+        <v>0</v>
+      </c>
+      <c r="C129" t="str">
+        <f>Source!C178</f>
+        <v>Shadowhand</v>
+      </c>
+      <c r="D129">
+        <f>Source!G178*Results!$B$5</f>
+        <v>80</v>
+      </c>
+      <c r="E129">
+        <f>Source!I178 * Results!$B$6</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" t="str">
+        <f>Source!A179</f>
+        <v>Terraformer</v>
+      </c>
+      <c r="B130">
+        <f>Source!B179</f>
+        <v>0</v>
+      </c>
+      <c r="C130">
+        <f>Source!C179</f>
+        <v>0</v>
+      </c>
+      <c r="D130">
+        <f>Source!G179*Results!$B$5</f>
+        <v>40</v>
+      </c>
+      <c r="E130">
+        <f>Source!I179 * Results!$B$6</f>
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Corrected build time, HP, and cost of expansion buildings and units.
</commit_message>
<xml_diff>
--- a/mods/dr/The Spreadsheet.xlsx
+++ b/mods/dr/The Spreadsheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539032E0-0F2D-4609-882F-0FF56AE62029}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0624606-85DC-4508-9C96-D3D69983BC3B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Source" sheetId="1" r:id="rId1"/>
@@ -2173,8 +2173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V179"/>
   <sheetViews>
-    <sheetView topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="A174" sqref="A174:XFD174"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3306,6 +3306,18 @@
       <c r="B46" t="s">
         <v>532</v>
       </c>
+      <c r="E46">
+        <v>750</v>
+      </c>
+      <c r="F46">
+        <v>8</v>
+      </c>
+      <c r="G46">
+        <v>1900</v>
+      </c>
+      <c r="H46">
+        <v>57</v>
+      </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -3313,6 +3325,18 @@
       </c>
       <c r="B47" t="s">
         <v>534</v>
+      </c>
+      <c r="E47">
+        <v>1400</v>
+      </c>
+      <c r="F47">
+        <v>8</v>
+      </c>
+      <c r="G47">
+        <v>1000</v>
+      </c>
+      <c r="H47">
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.25">
@@ -7888,8 +7912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD92D53-EC10-4CE0-957A-62D9B9206E5C}">
   <dimension ref="A1:G130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="A116" sqref="A116"/>
+    <sheetView topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="A136" sqref="A136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Disallowed rigs from building on water/taelon. Did a major pass over unit speeds. Stopped water/taelon from rendering above units. Fixed some icon issues. Disabled extraneous skirmish options. Nerfed AI.
</commit_message>
<xml_diff>
--- a/mods/dr/The Spreadsheet.xlsx
+++ b/mods/dr/The Spreadsheet.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0624606-85DC-4508-9C96-D3D69983BC3B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9634BA-D1AB-4D7E-A339-90663BC05095}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Source" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,18 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="575">
   <si>
     <t>Unit</t>
   </si>
@@ -1737,6 +1743,15 @@
   </si>
   <si>
     <t>Terraformer</t>
+  </si>
+  <si>
+    <t>Move Speed 2</t>
+  </si>
+  <si>
+    <t>Move speed multiplier</t>
+  </si>
+  <si>
+    <t>Move speed base</t>
   </si>
 </sst>
 </file>
@@ -2173,8 +2188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+    <sheetView topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="M111" sqref="M111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7910,10 +7925,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD92D53-EC10-4CE0-957A-62D9B9206E5C}">
-  <dimension ref="A1:G130"/>
+  <dimension ref="A1:P130"/>
   <sheetViews>
-    <sheetView topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="A136" sqref="A136"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="K119" sqref="K119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7921,20 +7936,28 @@
     <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" customWidth="1"/>
+    <col min="15" max="15" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>515</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O2" t="s">
+        <v>573</v>
+      </c>
+      <c r="P2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>527</v>
       </c>
@@ -7942,8 +7965,14 @@
         <f>1024/24</f>
         <v>42.666666666666664</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="O3" t="s">
+        <v>574</v>
+      </c>
+      <c r="P3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>525</v>
       </c>
@@ -7951,7 +7980,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>526</v>
       </c>
@@ -7959,7 +7988,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>528</v>
       </c>
@@ -7967,7 +7996,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>32</v>
       </c>
@@ -7990,7 +8019,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>Source!A52</f>
         <v>Chaff</v>
@@ -8020,7 +8049,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>Source!A53</f>
         <v>LaserRifle</v>
@@ -8050,7 +8079,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>Source!A54</f>
         <v>RailGun</v>
@@ -8080,7 +8109,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>Source!A55</f>
         <v>DoubleRailGun</v>
@@ -8110,7 +8139,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>Source!A56</f>
         <v>TripleRailGun</v>
@@ -8140,7 +8169,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>Source!A57</f>
         <v>SkirmishGun1</v>
@@ -8170,7 +8199,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>Source!A58</f>
         <v>SniperRifle</v>
@@ -8200,7 +8229,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>Source!A59</f>
         <v>PlasmaCannon</v>
@@ -9449,6 +9478,9 @@
       <c r="E60" s="7" t="s">
         <v>524</v>
       </c>
+      <c r="F60" s="7" t="s">
+        <v>572</v>
+      </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
@@ -9471,6 +9503,10 @@
         <f>Source!I110 * Results!$B$6</f>
         <v>72</v>
       </c>
+      <c r="F61">
+        <f>Source!I110 * Results!$P$2 + Results!$P$3</f>
+        <v>66</v>
+      </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
@@ -9493,6 +9529,10 @@
         <f>Source!I111 * Results!$B$6</f>
         <v>120</v>
       </c>
+      <c r="F62">
+        <f>Source!I111 * Results!$P$2 + Results!$P$3</f>
+        <v>90</v>
+      </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
@@ -9515,6 +9555,10 @@
         <f>Source!I112 * Results!$B$6</f>
         <v>192</v>
       </c>
+      <c r="F63">
+        <f>Source!I112 * Results!$P$2 + Results!$P$3</f>
+        <v>126</v>
+      </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
@@ -9537,8 +9581,12 @@
         <f>Source!I113 * Results!$B$6</f>
         <v>96</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64">
+        <f>Source!I113 * Results!$P$2 + Results!$P$3</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f>Source!A114</f>
         <v>FGMercenary</v>
@@ -9559,8 +9607,12 @@
         <f>Source!I114 * Results!$B$6</f>
         <v>96</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <f>Source!I114 * Results!$P$2 + Results!$P$3</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f>Source!A115</f>
         <v>FGSniper</v>
@@ -9581,8 +9633,12 @@
         <f>Source!I115 * Results!$B$6</f>
         <v>144</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <f>Source!I115 * Results!$P$2 + Results!$P$3</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f>Source!A116</f>
         <v>FGScout</v>
@@ -9603,8 +9659,12 @@
         <f>Source!I116 * Results!$B$6</f>
         <v>144</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F67">
+        <f>Source!I116 * Results!$P$2 + Results!$P$3</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f>Source!A117</f>
         <v>FGMedic</v>
@@ -9625,8 +9685,12 @@
         <f>Source!I117 * Results!$B$6</f>
         <v>96</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68">
+        <f>Source!I117 * Results!$P$2 + Results!$P$3</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
         <f>Source!A118</f>
         <v>FGSaboteur</v>
@@ -9647,8 +9711,12 @@
         <f>Source!I118 * Results!$B$6</f>
         <v>144</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69">
+        <f>Source!I118 * Results!$P$2 + Results!$P$3</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
         <f>Source!A119</f>
         <v>FGMechanic</v>
@@ -9669,8 +9737,12 @@
         <f>Source!I119 * Results!$B$6</f>
         <v>144</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <f>Source!I119 * Results!$P$2 + Results!$P$3</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
         <f>Source!A120</f>
         <v>FGSuicideNuker</v>
@@ -9691,8 +9763,12 @@
         <f>Source!I120 * Results!$B$6</f>
         <v>192</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F71">
+        <f>Source!I120 * Results!$P$2 + Results!$P$3</f>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
         <f>Source!A121</f>
         <v>FGSpy</v>
@@ -9713,8 +9789,12 @@
         <f>Source!I121 * Results!$B$6</f>
         <v>144</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F72">
+        <f>Source!I121 * Results!$P$2 + Results!$P$3</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
         <f>Source!A122</f>
         <v>FGSpiderBike</v>
@@ -9735,8 +9815,12 @@
         <f>Source!I122 * Results!$B$6</f>
         <v>288</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F73">
+        <f>Source!I122 * Results!$P$2 + Results!$P$3</f>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
         <f>Source!A123</f>
         <v>FGIFV</v>
@@ -9757,8 +9841,12 @@
         <f>Source!I123 * Results!$B$6</f>
         <v>216</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F74">
+        <f>Source!I123 * Results!$P$2 + Results!$P$3</f>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
         <f>Source!A124</f>
         <v>FGMediumTank</v>
@@ -9779,8 +9867,12 @@
         <f>Source!I124 * Results!$B$6</f>
         <v>192</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F75">
+        <f>Source!I124 * Results!$P$2 + Results!$P$3</f>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
         <f>Source!A125</f>
         <v>FGTankHunterTank</v>
@@ -9801,8 +9893,12 @@
         <f>Source!I125 * Results!$B$6</f>
         <v>240</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F76">
+        <f>Source!I125 * Results!$P$2 + Results!$P$3</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
         <f>Source!A126</f>
         <v>FGAmbushTank</v>
@@ -9823,8 +9919,12 @@
         <f>Source!I126 * Results!$B$6</f>
         <v>144</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F77">
+        <f>Source!I126 * Results!$P$2 + Results!$P$3</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="str">
         <f>Source!A127</f>
         <v>FGConstructionMAD</v>
@@ -9845,8 +9945,12 @@
         <f>Source!I127 * Results!$B$6</f>
         <v>144</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F78">
+        <f>Source!I127 * Results!$P$2 + Results!$P$3</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
         <f>Source!A128</f>
         <v>FGTripleRailHoverTank</v>
@@ -9867,8 +9971,12 @@
         <f>Source!I128 * Results!$B$6</f>
         <v>144</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F79">
+        <f>Source!I128 * Results!$P$2 + Results!$P$3</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="str">
         <f>Source!A129</f>
         <v>FGSPA</v>
@@ -9889,8 +9997,15 @@
         <f>Source!I129 * Results!$B$6</f>
         <v>96</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F80">
+        <f>Source!I129 * Results!$P$2 + Results!$P$3</f>
+        <v>78</v>
+      </c>
+      <c r="G80">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="str">
         <f>Source!A130</f>
         <v>FGSkyBike</v>
@@ -9911,8 +10026,12 @@
         <f>Source!I130 * Results!$B$6</f>
         <v>336</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F81">
+        <f>Source!I130 * Results!$P$2 + Results!$P$3</f>
+        <v>198</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="str">
         <f>Source!A131</f>
         <v>FGDualSkyBike</v>
@@ -9933,8 +10052,12 @@
         <f>Source!I131 * Results!$B$6</f>
         <v>288</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F82">
+        <f>Source!I131 * Results!$P$2 + Results!$P$3</f>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="str">
         <f>Source!A132</f>
         <v>FGShockWave</v>
@@ -9955,8 +10078,15 @@
         <f>Source!I132 * Results!$B$6</f>
         <v>96</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F83">
+        <f>Source!I132 * Results!$P$2 + Results!$P$3</f>
+        <v>78</v>
+      </c>
+      <c r="G83">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="str">
         <f>Source!A133</f>
         <v>FGContaminator</v>
@@ -9977,8 +10107,15 @@
         <f>Source!I133 * Results!$B$6</f>
         <v>48</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F84">
+        <f>Source!I133 * Results!$P$2 + Results!$P$3</f>
+        <v>54</v>
+      </c>
+      <c r="G84">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="str">
         <f>Source!A134</f>
         <v>FGundergtunnel</v>
@@ -9999,8 +10136,12 @@
         <f>Source!I134 * Results!$B$6</f>
         <v>96</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F85">
+        <f>Source!I134 * Results!$P$2 + Results!$P$3</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="str">
         <f>Source!A135</f>
         <v>FGAntiAirSite</v>
@@ -10021,8 +10162,12 @@
         <f>Source!I135 * Results!$B$6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F86">
+        <f>Source!I135 * Results!$P$2 + Results!$P$3</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="str">
         <f>Source!A136</f>
         <v>FGGuardTower</v>
@@ -10043,8 +10188,12 @@
         <f>Source!I136 * Results!$B$6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F87">
+        <f>Source!I136 * Results!$P$2 + Results!$P$3</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="str">
         <f>Source!A137</f>
         <v>FGAdvancedGuardTower</v>
@@ -10065,8 +10214,12 @@
         <f>Source!I137 * Results!$B$6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F88">
+        <f>Source!I137 * Results!$P$2 + Results!$P$3</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="str">
         <f>Source!A138</f>
         <v>FGBaseMover</v>
@@ -10087,8 +10240,12 @@
         <f>Source!I138 * Results!$B$6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F89">
+        <f>Source!I138 * Results!$P$2 + Results!$P$3</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="str">
         <f>Source!A139</f>
         <v>IMPConstructionCrew</v>
@@ -10109,8 +10266,12 @@
         <f>Source!I139 * Results!$B$6</f>
         <v>72</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F90">
+        <f>Source!I139 * Results!$P$2 + Results!$P$3</f>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="str">
         <f>Source!A140</f>
         <v>ImpGroundTransporter</v>
@@ -10131,8 +10292,12 @@
         <f>Source!I140 * Results!$B$6</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F91">
+        <f>Source!I140 * Results!$P$2 + Results!$P$3</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="str">
         <f>Source!A141</f>
         <v>ImpHoverTransporter</v>
@@ -10153,8 +10318,12 @@
         <f>Source!I141 * Results!$B$6</f>
         <v>192</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F92">
+        <f>Source!I141 * Results!$P$2 + Results!$P$3</f>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="str">
         <f>Source!A142</f>
         <v>IMPStrikeMarine</v>
@@ -10175,8 +10344,12 @@
         <f>Source!I142 * Results!$B$6</f>
         <v>96</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F93">
+        <f>Source!I142 * Results!$P$2 + Results!$P$3</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="str">
         <f>Source!A143</f>
         <v>IMPFireSupportMarine</v>
@@ -10197,8 +10370,12 @@
         <f>Source!I143 * Results!$B$6</f>
         <v>72</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F94">
+        <f>Source!I143 * Results!$P$2 + Results!$P$3</f>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="str">
         <f>Source!A144</f>
         <v>IMPHoverMarine</v>
@@ -10219,8 +10396,12 @@
         <f>Source!I144 * Results!$B$6</f>
         <v>192</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F95">
+        <f>Source!I144 * Results!$P$2 + Results!$P$3</f>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="str">
         <f>Source!A145</f>
         <v>IMPSpy</v>
@@ -10241,8 +10422,12 @@
         <f>Source!I145 * Results!$B$6</f>
         <v>144</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F96">
+        <f>Source!I145 * Results!$P$2 + Results!$P$3</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="str">
         <f>Source!A146</f>
         <v>IMPSuicideZombie</v>
@@ -10263,8 +10448,12 @@
         <f>Source!I146 * Results!$B$6</f>
         <v>72</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F97">
+        <f>Source!I146 * Results!$P$2 + Results!$P$3</f>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="str">
         <f>Source!A147</f>
         <v>IMPScoutTank</v>
@@ -10285,8 +10474,12 @@
         <f>Source!I147 * Results!$B$6</f>
         <v>240</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F98">
+        <f>Source!I147 * Results!$P$2 + Results!$P$3</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="str">
         <f>Source!A148</f>
         <v>IMPAssaultVehicle</v>
@@ -10307,8 +10500,12 @@
         <f>Source!I148 * Results!$B$6</f>
         <v>240</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F99">
+        <f>Source!I148 * Results!$P$2 + Results!$P$3</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="str">
         <f>Source!A149</f>
         <v>IMPPlasmaTank</v>
@@ -10329,8 +10526,12 @@
         <f>Source!I149 * Results!$B$6</f>
         <v>192</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F100">
+        <f>Source!I149 * Results!$P$2 + Results!$P$3</f>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="str">
         <f>Source!A150</f>
         <v>IMPAmper</v>
@@ -10351,8 +10552,12 @@
         <f>Source!I150 * Results!$B$6</f>
         <v>96</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F101">
+        <f>Source!I150 * Results!$P$2 + Results!$P$3</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="str">
         <f>Source!A151</f>
         <v>IMPMAD</v>
@@ -10373,8 +10578,12 @@
         <f>Source!I151 * Results!$B$6</f>
         <v>192</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F102">
+        <f>Source!I151 * Results!$P$2 + Results!$P$3</f>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="str">
         <f>Source!A152</f>
         <v>IMPReconSaucer</v>
@@ -10395,8 +10604,12 @@
         <f>Source!I152 * Results!$B$6</f>
         <v>192</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F103">
+        <f>Source!I152 * Results!$P$2 + Results!$P$3</f>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="str">
         <f>Source!A153</f>
         <v>IMPShredder</v>
@@ -10417,8 +10630,12 @@
         <f>Source!I153 * Results!$B$6</f>
         <v>240</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F104">
+        <f>Source!I153 * Results!$P$2 + Results!$P$3</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="str">
         <f>Source!A154</f>
         <v>IMPHostageTaker</v>
@@ -10439,8 +10656,12 @@
         <f>Source!I154 * Results!$B$6</f>
         <v>240</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F105">
+        <f>Source!I154 * Results!$P$2 + Results!$P$3</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="str">
         <f>Source!A155</f>
         <v>IMPTachyonTank</v>
@@ -10461,8 +10682,12 @@
         <f>Source!I155 * Results!$B$6</f>
         <v>144</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F106">
+        <f>Source!I155 * Results!$P$2 + Results!$P$3</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="str">
         <f>Source!A156</f>
         <v>IMPShieldedSPA</v>
@@ -10483,8 +10708,12 @@
         <f>Source!I156 * Results!$B$6</f>
         <v>144</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F107">
+        <f>Source!I156 * Results!$P$2 + Results!$P$3</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="str">
         <f>Source!A157</f>
         <v>IMPSPA</v>
@@ -10505,8 +10734,15 @@
         <f>Source!I157 * Results!$B$6</f>
         <v>72</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F108">
+        <f>Source!I157 * Results!$P$2 + Results!$P$3</f>
+        <v>66</v>
+      </c>
+      <c r="G108">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="str">
         <f>Source!A158</f>
         <v>ImpVTOL</v>
@@ -10527,8 +10763,12 @@
         <f>Source!I158 * Results!$B$6</f>
         <v>288</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F109">
+        <f>Source!I158 * Results!$P$2 + Results!$P$3</f>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="str">
         <f>Source!A159</f>
         <v>IMPSkyFortress</v>
@@ -10549,8 +10789,12 @@
         <f>Source!I159 * Results!$B$6</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F110">
+        <f>Source!I159 * Results!$P$2 + Results!$P$3</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="str">
         <f>Source!A160</f>
         <v>IMPContaminator</v>
@@ -10571,8 +10815,12 @@
         <f>Source!I160 * Results!$B$6</f>
         <v>48</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F111">
+        <f>Source!I160 * Results!$P$2 + Results!$P$3</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="str">
         <f>Source!A161</f>
         <v>IMPAntiAirSite</v>
@@ -10593,8 +10841,12 @@
         <f>Source!I161 * Results!$B$6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F112">
+        <f>Source!I161 * Results!$P$2 + Results!$P$3</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="str">
         <f>Source!A162</f>
         <v>IMPGuardTower</v>
@@ -10615,8 +10867,12 @@
         <f>Source!I162 * Results!$B$6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F113">
+        <f>Source!I162 * Results!$P$2 + Results!$P$3</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="str">
         <f>Source!A163</f>
         <v>IMPAdvancedGuardTower</v>
@@ -10637,8 +10893,12 @@
         <f>Source!I163 * Results!$B$6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F114">
+        <f>Source!I163 * Results!$P$2 + Results!$P$3</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="str">
         <f>Source!A164</f>
         <v>IMPriftCreator</v>
@@ -10659,8 +10919,12 @@
         <f>Source!I164 * Results!$B$6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F115">
+        <f>Source!I164 * Results!$P$2 + Results!$P$3</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="str">
         <f>Source!A165</f>
         <v>CameraTower</v>
@@ -10681,8 +10945,12 @@
         <f>Source!I165 * Results!$B$6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F116">
+        <f>Source!I165 * Results!$P$2 + Results!$P$3</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="str">
         <f>Source!A166</f>
         <v>Gant</v>
@@ -10703,8 +10971,12 @@
         <f>Source!I166 * Results!$B$6</f>
         <v>168</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F117">
+        <f>Source!I166 * Results!$P$2 + Results!$P$3</f>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="str">
         <f>Source!A167</f>
         <v>Ranger</v>
@@ -10725,8 +10997,12 @@
         <f>Source!I167 * Results!$B$6</f>
         <v>144</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F118">
+        <f>Source!I167 * Results!$P$2 + Results!$P$3</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="str">
         <f>Source!A168</f>
         <v>Grendel</v>
@@ -10747,8 +11023,12 @@
         <f>Source!I168 * Results!$B$6</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F119">
+        <f>Source!I168 * Results!$P$2 + Results!$P$3</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="str">
         <f>Source!A169</f>
         <v>Grendel Rider</v>
@@ -10769,8 +11049,12 @@
         <f>Source!I169 * Results!$B$6</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F120">
+        <f>Source!I169 * Results!$P$2 + Results!$P$3</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="str">
         <f>Source!A170</f>
         <v>Power Spiker</v>
@@ -10791,8 +11075,12 @@
         <f>Source!I170 * Results!$B$6</f>
         <v>96</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F121">
+        <f>Source!I170 * Results!$P$2 + Results!$P$3</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="str">
         <f>Source!A171</f>
         <v>Reaper</v>
@@ -10813,8 +11101,12 @@
         <f>Source!I171 * Results!$B$6</f>
         <v>96</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F122">
+        <f>Source!I171 * Results!$P$2 + Results!$P$3</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="str">
         <f>Source!A172</f>
         <v>Fury</v>
@@ -10835,8 +11127,12 @@
         <f>Source!I172 * Results!$B$6</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F123">
+        <f>Source!I172 * Results!$P$2 + Results!$P$3</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="str">
         <f>Source!A173</f>
         <v>Hades Bomber</v>
@@ -10857,8 +11153,12 @@
         <f>Source!I173 * Results!$B$6</f>
         <v>240</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F124">
+        <f>Source!I173 * Results!$P$2 + Results!$P$3</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="str">
         <f>Source!A174</f>
         <v>Avenger</v>
@@ -10879,8 +11179,12 @@
         <f>Source!I174 * Results!$B$6</f>
         <v>216</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F125">
+        <f>Source!I174 * Results!$P$2 + Results!$P$3</f>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="str">
         <f>Source!A175</f>
         <v>EMP</v>
@@ -10901,8 +11205,12 @@
         <f>Source!I175 * Results!$B$6</f>
         <v>144</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F126">
+        <f>Source!I175 * Results!$P$2 + Results!$P$3</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="str">
         <f>Source!A176</f>
         <v>Ratmk2</v>
@@ -10923,8 +11231,12 @@
         <f>Source!I176 * Results!$B$6</f>
         <v>216</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F127">
+        <f>Source!I176 * Results!$P$2 + Results!$P$3</f>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="str">
         <f>Source!A177</f>
         <v>GeminiTank</v>
@@ -10945,8 +11257,12 @@
         <f>Source!I177 * Results!$B$6</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F128">
+        <f>Source!I177 * Results!$P$2 + Results!$P$3</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="str">
         <f>Source!A178</f>
         <v>Shadowblade</v>
@@ -10967,8 +11283,12 @@
         <f>Source!I178 * Results!$B$6</f>
         <v>240</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F129">
+        <f>Source!I178 * Results!$P$2 + Results!$P$3</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="str">
         <f>Source!A179</f>
         <v>Terraformer</v>
@@ -10988,6 +11308,10 @@
       <c r="E130">
         <f>Source!I179 * Results!$B$6</f>
         <v>96</v>
+      </c>
+      <c r="F130">
+        <f>Source!I179 * Results!$P$2 + Results!$P$3</f>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>